<commit_message>
US 39 & 42 and Updated Report
Checks for anniversaries and reject dates that cannot be converted to a datetime object.
</commit_message>
<xml_diff>
--- a/Team05Report.xlsx
+++ b/Team05Report.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22228"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\samar\Downloads\Scanned pics\New\Assignments\Agile\Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Apostolico\Documents\2019fall-Group5-555B-Project-master(1)\2019fall-Group5-555B-Project-master\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEFC0C45-35E1-4772-862A-228415ED589B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{152AD873-77C7-49D0-8B97-ACE5BA40032B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
@@ -42,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="596" uniqueCount="223">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="606" uniqueCount="229">
   <si>
     <t>Date</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -822,6 +824,24 @@
   </si>
   <si>
     <t>Coding</t>
+  </si>
+  <si>
+    <t>US41</t>
+  </si>
+  <si>
+    <t>Include Partial Dates</t>
+  </si>
+  <si>
+    <t>US42</t>
+  </si>
+  <si>
+    <t>Reject Illegitimate Dates</t>
+  </si>
+  <si>
+    <t>Reject Illegitimate dates</t>
+  </si>
+  <si>
+    <t>Done</t>
   </si>
 </sst>
 </file>
@@ -2220,12 +2240,12 @@
       <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.6"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="7.81640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18" customWidth="1"/>
-    <col min="3" max="3" width="8.453125" customWidth="1"/>
-    <col min="4" max="5" width="20.453125" customWidth="1"/>
+    <col min="3" max="3" width="8.5" customWidth="1"/>
+    <col min="4" max="5" width="20.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="4" customFormat="1">
@@ -2373,19 +2393,19 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:E41"/>
+  <dimension ref="A1:E43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="150" workbookViewId="0">
-      <selection activeCell="G28" sqref="G28"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="150" workbookViewId="0">
+      <selection activeCell="E43" sqref="E43"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.6"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="5.1796875" customWidth="1"/>
-    <col min="2" max="2" width="9.6328125" customWidth="1"/>
+    <col min="1" max="1" width="5.125" customWidth="1"/>
+    <col min="2" max="2" width="9.625" customWidth="1"/>
     <col min="3" max="3" width="31" customWidth="1"/>
-    <col min="4" max="4" width="6.6328125" customWidth="1"/>
-    <col min="5" max="5" width="7.6328125" customWidth="1"/>
+    <col min="4" max="4" width="6.625" customWidth="1"/>
+    <col min="5" max="5" width="7.625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="4" customFormat="1">
@@ -3065,7 +3085,7 @@
         <v>172</v>
       </c>
       <c r="E40" s="16" t="s">
-        <v>204</v>
+        <v>228</v>
       </c>
     </row>
     <row r="41" spans="1:5">
@@ -3083,6 +3103,40 @@
       </c>
       <c r="E41" s="16" t="s">
         <v>204</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5">
+      <c r="A42">
+        <v>41</v>
+      </c>
+      <c r="B42" s="16" t="s">
+        <v>223</v>
+      </c>
+      <c r="C42" t="s">
+        <v>224</v>
+      </c>
+      <c r="D42" t="s">
+        <v>172</v>
+      </c>
+      <c r="E42" s="16" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5">
+      <c r="A43">
+        <v>42</v>
+      </c>
+      <c r="B43" s="16" t="s">
+        <v>225</v>
+      </c>
+      <c r="C43" t="s">
+        <v>226</v>
+      </c>
+      <c r="D43" t="s">
+        <v>172</v>
+      </c>
+      <c r="E43" t="s">
+        <v>228</v>
       </c>
     </row>
   </sheetData>
@@ -3100,14 +3154,14 @@
       <selection activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.6"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="10.81640625" style="7"/>
-    <col min="2" max="2" width="9.453125" customWidth="1"/>
-    <col min="3" max="3" width="15.81640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.36328125" customWidth="1"/>
-    <col min="5" max="5" width="6.81640625" customWidth="1"/>
-    <col min="6" max="6" width="12.453125" style="9" customWidth="1"/>
+    <col min="1" max="1" width="10.875" style="7"/>
+    <col min="2" max="2" width="9.5" customWidth="1"/>
+    <col min="3" max="3" width="15.875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.375" customWidth="1"/>
+    <col min="5" max="5" width="6.875" customWidth="1"/>
+    <col min="6" max="6" width="12.5" style="9" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -3295,14 +3349,14 @@
       <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.6"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="10.81640625" style="2"/>
-    <col min="2" max="2" width="24.453125" customWidth="1"/>
-    <col min="3" max="3" width="17.81640625" customWidth="1"/>
-    <col min="4" max="4" width="11.1796875" customWidth="1"/>
-    <col min="5" max="5" width="13.6328125" customWidth="1"/>
-    <col min="6" max="6" width="12.453125" style="9" customWidth="1"/>
+    <col min="1" max="1" width="10.875" style="2"/>
+    <col min="2" max="2" width="24.5" customWidth="1"/>
+    <col min="3" max="3" width="17.875" customWidth="1"/>
+    <col min="4" max="4" width="11.125" customWidth="1"/>
+    <col min="5" max="5" width="13.625" customWidth="1"/>
+    <col min="6" max="6" width="12.5" style="9" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" s="4" customFormat="1">
@@ -3416,17 +3470,17 @@
       <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.6"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="7.6328125" customWidth="1"/>
-    <col min="2" max="2" width="24.453125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="12.6328125" customWidth="1"/>
-    <col min="4" max="4" width="20.81640625" customWidth="1"/>
-    <col min="5" max="5" width="14.6328125" customWidth="1"/>
-    <col min="6" max="6" width="11.81640625" customWidth="1"/>
-    <col min="7" max="7" width="12.81640625" customWidth="1"/>
+    <col min="1" max="1" width="7.625" customWidth="1"/>
+    <col min="2" max="2" width="24.5" style="1" customWidth="1"/>
+    <col min="3" max="3" width="12.625" customWidth="1"/>
+    <col min="4" max="4" width="20.875" customWidth="1"/>
+    <col min="5" max="5" width="14.625" customWidth="1"/>
+    <col min="6" max="6" width="11.875" customWidth="1"/>
+    <col min="7" max="7" width="12.875" customWidth="1"/>
     <col min="8" max="8" width="18" customWidth="1"/>
-    <col min="9" max="9" width="10.81640625" style="6"/>
+    <col min="9" max="9" width="10.875" style="6"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
@@ -3661,7 +3715,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="25.2">
+    <row r="9" spans="1:9" ht="25.5">
       <c r="A9" t="s">
         <v>115</v>
       </c>
@@ -3799,12 +3853,12 @@
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.6"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75"/>
   <cols>
-    <col min="2" max="2" width="28.1796875" customWidth="1"/>
+    <col min="2" max="2" width="28.125" customWidth="1"/>
     <col min="5" max="5" width="14" customWidth="1"/>
-    <col min="6" max="6" width="14.1796875" customWidth="1"/>
-    <col min="7" max="7" width="13.453125" customWidth="1"/>
+    <col min="6" max="6" width="14.125" customWidth="1"/>
+    <col min="7" max="7" width="13.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
@@ -4175,13 +4229,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:I21"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" zoomScale="150" workbookViewId="0">
+    <sheetView zoomScale="150" workbookViewId="0">
       <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.6"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75"/>
   <cols>
-    <col min="2" max="2" width="38.08984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="38.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
@@ -4552,12 +4606,12 @@
   <dimension ref="A1:I20"/>
   <sheetViews>
     <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.6"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75"/>
   <cols>
-    <col min="2" max="2" width="28.81640625" customWidth="1"/>
+    <col min="2" max="2" width="28.875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
@@ -4768,13 +4822,22 @@
       <c r="F10">
         <v>20</v>
       </c>
+      <c r="G10">
+        <v>20</v>
+      </c>
+      <c r="H10">
+        <v>15</v>
+      </c>
+      <c r="I10" t="s">
+        <v>228</v>
+      </c>
     </row>
     <row r="11" spans="1:9">
       <c r="A11" s="16" t="s">
-        <v>147</v>
+        <v>225</v>
       </c>
       <c r="B11" t="s">
-        <v>104</v>
+        <v>227</v>
       </c>
       <c r="C11" t="s">
         <v>172</v>
@@ -4787,6 +4850,15 @@
       </c>
       <c r="F11">
         <v>20</v>
+      </c>
+      <c r="G11">
+        <v>10</v>
+      </c>
+      <c r="H11">
+        <v>10</v>
+      </c>
+      <c r="I11" t="s">
+        <v>228</v>
       </c>
     </row>
     <row r="13" spans="1:9">
@@ -4833,10 +4905,10 @@
       <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.6"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75"/>
   <cols>
-    <col min="2" max="2" width="37.54296875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="68.453125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="37.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="68.5" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" s="4" customFormat="1">
@@ -4850,7 +4922,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="15">
+    <row r="2" spans="1:3" ht="31.5">
       <c r="A2" s="17" t="s">
         <v>108</v>
       </c>
@@ -4861,7 +4933,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="15">
+    <row r="3" spans="1:3" ht="15.75">
       <c r="A3" s="17" t="s">
         <v>109</v>
       </c>
@@ -4872,7 +4944,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="15">
+    <row r="4" spans="1:3" ht="15.75">
       <c r="A4" t="s">
         <v>110</v>
       </c>
@@ -4883,7 +4955,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="30">
+    <row r="5" spans="1:3" ht="31.5">
       <c r="A5" t="s">
         <v>111</v>
       </c>
@@ -4894,7 +4966,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="15">
+    <row r="6" spans="1:3" ht="15.75">
       <c r="A6" t="s">
         <v>112</v>
       </c>
@@ -4905,7 +4977,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="15">
+    <row r="7" spans="1:3" ht="15.75">
       <c r="A7" t="s">
         <v>113</v>
       </c>
@@ -4916,7 +4988,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="30">
+    <row r="8" spans="1:3" ht="31.5">
       <c r="A8" t="s">
         <v>114</v>
       </c>
@@ -4927,7 +4999,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="30">
+    <row r="9" spans="1:3" ht="31.5">
       <c r="A9" t="s">
         <v>115</v>
       </c>
@@ -4938,7 +5010,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="30">
+    <row r="10" spans="1:3" ht="31.5">
       <c r="A10" t="s">
         <v>116</v>
       </c>
@@ -4949,7 +5021,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="30">
+    <row r="11" spans="1:3" ht="31.5">
       <c r="A11" t="s">
         <v>117</v>
       </c>
@@ -4960,7 +5032,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="15">
+    <row r="12" spans="1:3" ht="15.75">
       <c r="A12" s="17" t="s">
         <v>118</v>
       </c>
@@ -4971,7 +5043,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="30">
+    <row r="13" spans="1:3" ht="31.5">
       <c r="A13" s="17" t="s">
         <v>119</v>
       </c>
@@ -4982,7 +5054,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="45">
+    <row r="14" spans="1:3" ht="47.25">
       <c r="A14" t="s">
         <v>120</v>
       </c>
@@ -4993,7 +5065,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="15">
+    <row r="15" spans="1:3" ht="15.75">
       <c r="A15" t="s">
         <v>121</v>
       </c>
@@ -5004,7 +5076,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="15">
+    <row r="16" spans="1:3" ht="15.75">
       <c r="A16" t="s">
         <v>122</v>
       </c>
@@ -5015,7 +5087,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="15">
+    <row r="17" spans="1:3" ht="15.75">
       <c r="A17" t="s">
         <v>123</v>
       </c>
@@ -5026,7 +5098,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="15">
+    <row r="18" spans="1:3" ht="15.75">
       <c r="A18" t="s">
         <v>124</v>
       </c>
@@ -5037,7 +5109,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="15">
+    <row r="19" spans="1:3" ht="15.75">
       <c r="A19" t="s">
         <v>125</v>
       </c>
@@ -5048,7 +5120,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="15">
+    <row r="20" spans="1:3" ht="15.75">
       <c r="A20" t="s">
         <v>126</v>
       </c>
@@ -5059,7 +5131,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="15">
+    <row r="21" spans="1:3" ht="15.75">
       <c r="A21" t="s">
         <v>127</v>
       </c>
@@ -5070,7 +5142,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="15">
+    <row r="22" spans="1:3" ht="15.75">
       <c r="A22" s="17" t="s">
         <v>128</v>
       </c>
@@ -5081,7 +5153,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="15">
+    <row r="23" spans="1:3" ht="15.75">
       <c r="A23" s="17" t="s">
         <v>129</v>
       </c>
@@ -5092,7 +5164,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="30">
+    <row r="24" spans="1:3" ht="31.5">
       <c r="A24" t="s">
         <v>130</v>
       </c>
@@ -5103,7 +5175,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="30">
+    <row r="25" spans="1:3" ht="31.5">
       <c r="A25" t="s">
         <v>131</v>
       </c>
@@ -5114,7 +5186,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="15">
+    <row r="26" spans="1:3" ht="15.75">
       <c r="A26" t="s">
         <v>132</v>
       </c>
@@ -5125,7 +5197,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="75">
+    <row r="27" spans="1:3" ht="78.75">
       <c r="A27" t="s">
         <v>133</v>
       </c>
@@ -5136,7 +5208,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="15">
+    <row r="28" spans="1:3" ht="15.75">
       <c r="A28" t="s">
         <v>134</v>
       </c>
@@ -5147,7 +5219,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="15">
+    <row r="29" spans="1:3" ht="15.75">
       <c r="A29" t="s">
         <v>135</v>
       </c>
@@ -5158,7 +5230,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="15">
+    <row r="30" spans="1:3" ht="15.75">
       <c r="A30" t="s">
         <v>136</v>
       </c>
@@ -5169,7 +5241,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="15">
+    <row r="31" spans="1:3" ht="15.75">
       <c r="A31" t="s">
         <v>137</v>
       </c>
@@ -5180,7 +5252,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="15">
+    <row r="32" spans="1:3" ht="31.5">
       <c r="A32" s="17" t="s">
         <v>138</v>
       </c>
@@ -5191,7 +5263,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="15">
+    <row r="33" spans="1:3" ht="15.75">
       <c r="A33" s="17" t="s">
         <v>139</v>
       </c>
@@ -5202,7 +5274,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="34" spans="1:3" ht="30">
+    <row r="34" spans="1:3" ht="31.5">
       <c r="A34" t="s">
         <v>140</v>
       </c>
@@ -5213,7 +5285,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="35" spans="1:3" ht="30">
+    <row r="35" spans="1:3" ht="31.5">
       <c r="A35" t="s">
         <v>141</v>
       </c>
@@ -5224,7 +5296,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="36" spans="1:3" ht="15">
+    <row r="36" spans="1:3" ht="15.75">
       <c r="A36" t="s">
         <v>142</v>
       </c>
@@ -5235,7 +5307,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="37" spans="1:3" ht="15">
+    <row r="37" spans="1:3" ht="15.75">
       <c r="A37" t="s">
         <v>143</v>
       </c>
@@ -5246,7 +5318,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="38" spans="1:3" ht="30">
+    <row r="38" spans="1:3" ht="31.5">
       <c r="A38" t="s">
         <v>144</v>
       </c>
@@ -5257,7 +5329,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="39" spans="1:3" ht="15">
+    <row r="39" spans="1:3" ht="31.5">
       <c r="A39" t="s">
         <v>145</v>
       </c>
@@ -5268,7 +5340,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="40" spans="1:3" ht="30">
+    <row r="40" spans="1:3" ht="31.5">
       <c r="A40" t="s">
         <v>146</v>
       </c>
@@ -5279,7 +5351,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="41" spans="1:3" ht="15">
+    <row r="41" spans="1:3" ht="15.75">
       <c r="A41" t="s">
         <v>147</v>
       </c>
@@ -5290,10 +5362,10 @@
         <v>105</v>
       </c>
     </row>
-    <row r="42" spans="1:3" ht="15">
+    <row r="42" spans="1:3" ht="15.75">
       <c r="C42" s="12"/>
     </row>
-    <row r="43" spans="1:3" ht="15">
+    <row r="43" spans="1:3" ht="15.75">
       <c r="C43" s="12"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
All finished team report
</commit_message>
<xml_diff>
--- a/Team05Report.xlsx
+++ b/Team05Report.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11110"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\samar\Downloads\Scanned pics\New\Assignments\Agile\Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ruohuanxu/Downloads/2019fall-Group5-555B-Project-master 3/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEFC0C45-35E1-4772-862A-228415ED589B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E39812EA-D2BA-3048-AF02-A34946943307}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="15460" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="596" uniqueCount="223">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="610" uniqueCount="221">
   <si>
     <t>Date</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -231,6 +231,9 @@
     <t>No more than one family with the same spouses by name and the same marriage date should appear in a GEDCOM file</t>
   </si>
   <si>
+    <t>No more than one child with the same name and birth date should appear in a family</t>
+  </si>
+  <si>
     <t>Include person's current age when listing individuals</t>
   </si>
   <si>
@@ -346,6 +349,9 @@
   </si>
   <si>
     <t>Unique families by spouses</t>
+  </si>
+  <si>
+    <t>Unique first names in families</t>
   </si>
   <si>
     <t>Corresponding entries</t>
@@ -752,10 +758,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>Coding</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>Done</t>
     <phoneticPr fontId="6" type="noConversion"/>
   </si>
@@ -808,20 +810,12 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>Coding</t>
+    <t>List living single</t>
     <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
-    <t>Unique child names in families</t>
-  </si>
-  <si>
-    <t>No more than one child with the same name should appear in a family</t>
-  </si>
-  <si>
-    <t>Unique child first names in families</t>
-  </si>
-  <si>
-    <t>Coding</t>
+    <t>List multiple births</t>
+    <phoneticPr fontId="6" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -829,8 +823,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="m/d"/>
-    <numFmt numFmtId="165" formatCode="0.0"/>
+    <numFmt numFmtId="176" formatCode="m/d"/>
+    <numFmt numFmtId="177" formatCode="0.0"/>
   </numFmts>
   <fonts count="13">
     <font>
@@ -1008,20 +1002,20 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="176" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="177" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -1029,7 +1023,7 @@
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="177" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1042,79 +1036,79 @@
     <xf numFmtId="49" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="65" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="176" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="66">
-    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="64" builtinId="9" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="59" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="61" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="63" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="65" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="超链接" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="49" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="51" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="53" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="55" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="57" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="59" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="61" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="63" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="65" builtinId="8"/>
+    <cellStyle name="已访问的超链接" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="58" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="60" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="62" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="64" builtinId="9" hidden="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
@@ -1132,7 +1126,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="1"/>
-  <c:lang val="en-US"/>
+  <c:lang val="zh-CN"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1156,7 +1150,7 @@
             <c:numRef>
               <c:f>'Burndown README'!$B$15:$B$20</c:f>
               <c:numCache>
-                <c:formatCode>m/d/yyyy</c:formatCode>
+                <c:formatCode>m/d/yy</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>41065</c:v>
@@ -1227,7 +1221,7 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:numFmt formatCode="m/d/yyyy" sourceLinked="1"/>
+        <c:numFmt formatCode="m/d/yy" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1269,7 +1263,7 @@
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="1"/>
-  <c:lang val="en-US"/>
+  <c:lang val="zh-CN"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1307,6 +1301,9 @@
                 <c:pt idx="3">
                   <c:v>42313</c:v>
                 </c:pt>
+                <c:pt idx="4">
+                  <c:v>42327</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
@@ -1327,6 +1324,9 @@
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2216,16 +2216,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G10"/>
   <sheetViews>
-    <sheetView zoomScale="150" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
       <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.6"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13"/>
   <cols>
-    <col min="1" max="1" width="7.81640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.83203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18" customWidth="1"/>
-    <col min="3" max="3" width="8.453125" customWidth="1"/>
-    <col min="4" max="5" width="20.453125" customWidth="1"/>
+    <col min="3" max="3" width="8.5" customWidth="1"/>
+    <col min="4" max="5" width="20.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="4" customFormat="1">
@@ -2247,87 +2247,87 @@
     </row>
     <row r="2" spans="1:7">
       <c r="A2" s="20" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="B2" s="20" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="C2" s="20" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="D2" s="21" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="E2" s="20" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" s="20" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="B3" s="20" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="C3" s="20" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="D3" s="21" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="E3" s="20" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
     </row>
     <row r="4" spans="1:7">
       <c r="A4" s="20" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="B4" s="20" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="C4" s="20" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="D4" s="21" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="E4" s="20" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
     </row>
     <row r="5" spans="1:7">
       <c r="A5" s="20" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="B5" s="20" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="C5" s="20" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="D5" s="21" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="E5" s="20" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c r="A6" s="20" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="B6" s="20" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="C6" s="20" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="D6" s="21" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="E6" s="20" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -2338,17 +2338,17 @@
         <v>35</v>
       </c>
       <c r="E9" s="21" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="F9" s="24"/>
       <c r="G9" s="24"/>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:7" ht="14">
       <c r="D10" s="24" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="E10" s="25" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="F10" s="24"/>
       <c r="G10" s="24"/>
@@ -2375,17 +2375,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="150" workbookViewId="0">
-      <selection activeCell="G28" sqref="G28"/>
+    <sheetView topLeftCell="A37" zoomScale="150" workbookViewId="0">
+      <selection activeCell="H40" sqref="H40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.6"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13"/>
   <cols>
-    <col min="1" max="1" width="5.1796875" customWidth="1"/>
-    <col min="2" max="2" width="9.6328125" customWidth="1"/>
+    <col min="1" max="1" width="5.1640625" customWidth="1"/>
+    <col min="2" max="2" width="9.6640625" customWidth="1"/>
     <col min="3" max="3" width="31" customWidth="1"/>
-    <col min="4" max="4" width="6.6328125" customWidth="1"/>
-    <col min="5" max="5" width="7.6328125" customWidth="1"/>
+    <col min="4" max="4" width="6.6640625" customWidth="1"/>
+    <col min="5" max="5" width="7.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="4" customFormat="1">
@@ -2410,13 +2410,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="16" t="s">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="C2" s="17" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="D2" s="16" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="E2" t="s">
         <v>29</v>
@@ -2427,13 +2427,13 @@
         <v>2</v>
       </c>
       <c r="B3" s="16" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
       <c r="C3" s="17" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D3" s="16" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="E3" t="s">
         <v>29</v>
@@ -2444,13 +2444,13 @@
         <v>3</v>
       </c>
       <c r="B4" s="16" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
       <c r="C4" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="D4" s="16" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="E4" t="s">
         <v>29</v>
@@ -2461,13 +2461,13 @@
         <v>4</v>
       </c>
       <c r="B5" s="16" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="C5" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D5" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="E5" t="s">
         <v>29</v>
@@ -2478,13 +2478,13 @@
         <v>5</v>
       </c>
       <c r="B6" s="16" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="C6" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D6" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="E6" t="s">
         <v>29</v>
@@ -2495,13 +2495,13 @@
         <v>6</v>
       </c>
       <c r="B7" s="16" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="C7" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D7" s="16" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="E7" t="s">
         <v>29</v>
@@ -2512,13 +2512,13 @@
         <v>7</v>
       </c>
       <c r="B8" s="16" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="C8" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="D8" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="E8" t="s">
         <v>29</v>
@@ -2529,13 +2529,13 @@
         <v>8</v>
       </c>
       <c r="B9" s="16" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="C9" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="D9" s="16" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="E9" t="s">
         <v>29</v>
@@ -2546,13 +2546,13 @@
         <v>9</v>
       </c>
       <c r="B10" s="16" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="C10" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D10" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="E10" t="s">
         <v>29</v>
@@ -2563,13 +2563,13 @@
         <v>10</v>
       </c>
       <c r="B11" s="16" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="C11" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D11" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="E11" t="s">
         <v>29</v>
@@ -2580,13 +2580,13 @@
         <v>11</v>
       </c>
       <c r="B12" s="16" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="C12" s="17" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D12" s="16" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="E12" t="s">
         <v>29</v>
@@ -2597,13 +2597,13 @@
         <v>12</v>
       </c>
       <c r="B13" s="16" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="C13" s="17" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="D13" s="16" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="E13" t="s">
         <v>29</v>
@@ -2614,13 +2614,13 @@
         <v>13</v>
       </c>
       <c r="B14" s="16" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="C14" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="D14" s="16" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="E14" t="s">
         <v>29</v>
@@ -2631,13 +2631,13 @@
         <v>14</v>
       </c>
       <c r="B15" s="16" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="C15" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="D15" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="E15" t="s">
         <v>29</v>
@@ -2648,13 +2648,13 @@
         <v>15</v>
       </c>
       <c r="B16" s="16" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="C16" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="D16" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="E16" t="s">
         <v>29</v>
@@ -2665,13 +2665,13 @@
         <v>16</v>
       </c>
       <c r="B17" s="16" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="C17" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="D17" s="16" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="E17" t="s">
         <v>29</v>
@@ -2682,13 +2682,13 @@
         <v>17</v>
       </c>
       <c r="B18" s="16" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="C18" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="D18" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="E18" t="s">
         <v>29</v>
@@ -2699,13 +2699,13 @@
         <v>18</v>
       </c>
       <c r="B19" s="16" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="C19" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="D19" s="16" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="E19" t="s">
         <v>29</v>
@@ -2716,13 +2716,13 @@
         <v>19</v>
       </c>
       <c r="B20" s="16" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="C20" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D20" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="E20" t="s">
         <v>29</v>
@@ -2733,13 +2733,13 @@
         <v>20</v>
       </c>
       <c r="B21" s="16" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="C21" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="D21" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="E21" t="s">
         <v>29</v>
@@ -2750,13 +2750,13 @@
         <v>21</v>
       </c>
       <c r="B22" s="16" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="C22" s="17" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="D22" s="16" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="E22" t="s">
         <v>29</v>
@@ -2767,13 +2767,13 @@
         <v>22</v>
       </c>
       <c r="B23" s="16" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="C23" s="19" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="D23" s="16" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="E23" t="s">
         <v>29</v>
@@ -2784,13 +2784,13 @@
         <v>23</v>
       </c>
       <c r="B24" s="16" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="C24" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="D24" s="16" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="E24" t="s">
         <v>29</v>
@@ -2801,13 +2801,13 @@
         <v>24</v>
       </c>
       <c r="B25" s="16" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="C25" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="D25" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="E25" t="s">
         <v>29</v>
@@ -2818,13 +2818,13 @@
         <v>25</v>
       </c>
       <c r="B26" s="16" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="C26" t="s">
-        <v>221</v>
+        <v>92</v>
       </c>
       <c r="D26" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="E26" t="s">
         <v>29</v>
@@ -2835,16 +2835,16 @@
         <v>26</v>
       </c>
       <c r="B27" s="16" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="C27" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="D27" s="16" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="E27" t="s">
-        <v>222</v>
+        <v>29</v>
       </c>
     </row>
     <row r="28" spans="1:5">
@@ -2852,13 +2852,13 @@
         <v>27</v>
       </c>
       <c r="B28" s="16" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="C28" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="D28" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="E28" t="s">
         <v>29</v>
@@ -2869,13 +2869,13 @@
         <v>28</v>
       </c>
       <c r="B29" s="16" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="C29" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="D29" s="16" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="E29" t="s">
         <v>29</v>
@@ -2886,13 +2886,13 @@
         <v>29</v>
       </c>
       <c r="B30" s="16" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="C30" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="D30" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="E30" t="s">
         <v>29</v>
@@ -2903,13 +2903,13 @@
         <v>30</v>
       </c>
       <c r="B31" s="16" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="C31" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="D31" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="E31" t="s">
         <v>29</v>
@@ -2920,16 +2920,16 @@
         <v>31</v>
       </c>
       <c r="B32" s="16" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="C32" s="17" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="D32" s="16" t="s">
-        <v>173</v>
-      </c>
-      <c r="E32" s="16" t="s">
-        <v>204</v>
+        <v>175</v>
+      </c>
+      <c r="E32" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="33" spans="1:5">
@@ -2937,16 +2937,16 @@
         <v>32</v>
       </c>
       <c r="B33" s="16" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="C33" s="17" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="D33" s="16" t="s">
-        <v>169</v>
-      </c>
-      <c r="E33" s="16" t="s">
-        <v>204</v>
+        <v>171</v>
+      </c>
+      <c r="E33" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="34" spans="1:5">
@@ -2954,16 +2954,16 @@
         <v>33</v>
       </c>
       <c r="B34" s="16" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="C34" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="D34" s="16" t="s">
-        <v>170</v>
-      </c>
-      <c r="E34" s="16" t="s">
-        <v>204</v>
+        <v>172</v>
+      </c>
+      <c r="E34" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="35" spans="1:5">
@@ -2971,16 +2971,16 @@
         <v>34</v>
       </c>
       <c r="B35" s="16" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="C35" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="D35" t="s">
-        <v>170</v>
-      </c>
-      <c r="E35" s="16" t="s">
-        <v>204</v>
+        <v>172</v>
+      </c>
+      <c r="E35" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="36" spans="1:5">
@@ -2988,16 +2988,16 @@
         <v>35</v>
       </c>
       <c r="B36" s="16" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="C36" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="D36" t="s">
-        <v>171</v>
-      </c>
-      <c r="E36" s="16" t="s">
-        <v>204</v>
+        <v>173</v>
+      </c>
+      <c r="E36" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="37" spans="1:5">
@@ -3005,16 +3005,16 @@
         <v>36</v>
       </c>
       <c r="B37" s="16" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="C37" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="D37" s="16" t="s">
-        <v>174</v>
-      </c>
-      <c r="E37" s="16" t="s">
-        <v>204</v>
+        <v>176</v>
+      </c>
+      <c r="E37" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="38" spans="1:5">
@@ -3022,16 +3022,16 @@
         <v>37</v>
       </c>
       <c r="B38" s="16" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="C38" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="D38" t="s">
-        <v>168</v>
-      </c>
-      <c r="E38" s="16" t="s">
-        <v>204</v>
+        <v>170</v>
+      </c>
+      <c r="E38" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="39" spans="1:5">
@@ -3039,16 +3039,16 @@
         <v>38</v>
       </c>
       <c r="B39" s="16" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="C39" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="D39" s="16" t="s">
-        <v>175</v>
-      </c>
-      <c r="E39" s="16" t="s">
-        <v>204</v>
+        <v>177</v>
+      </c>
+      <c r="E39" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="40" spans="1:5">
@@ -3056,16 +3056,16 @@
         <v>39</v>
       </c>
       <c r="B40" s="16" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="C40" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="D40" t="s">
-        <v>172</v>
-      </c>
-      <c r="E40" s="16" t="s">
-        <v>204</v>
+        <v>174</v>
+      </c>
+      <c r="E40" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="41" spans="1:5">
@@ -3073,16 +3073,16 @@
         <v>40</v>
       </c>
       <c r="B41" s="16" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="C41" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="D41" t="s">
-        <v>172</v>
-      </c>
-      <c r="E41" s="16" t="s">
-        <v>204</v>
+        <v>174</v>
+      </c>
+      <c r="E41" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -3100,49 +3100,49 @@
       <selection activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.6"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13"/>
   <cols>
-    <col min="1" max="1" width="10.81640625" style="7"/>
-    <col min="2" max="2" width="9.453125" customWidth="1"/>
-    <col min="3" max="3" width="15.81640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.36328125" customWidth="1"/>
-    <col min="5" max="5" width="6.81640625" customWidth="1"/>
-    <col min="6" max="6" width="12.453125" style="9" customWidth="1"/>
+    <col min="1" max="1" width="10.83203125" style="7"/>
+    <col min="2" max="2" width="9.5" customWidth="1"/>
+    <col min="3" max="3" width="15.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.33203125" customWidth="1"/>
+    <col min="5" max="5" width="6.83203125" customWidth="1"/>
+    <col min="6" max="6" width="12.5" style="9" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" s="7" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
     </row>
     <row r="2" spans="1:7">
       <c r="A2" s="7" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" s="7" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
     </row>
     <row r="5" spans="1:7">
       <c r="A5" s="7" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c r="A6" s="7" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="7" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
     </row>
     <row r="14" spans="1:7" s="4" customFormat="1">
       <c r="A14" s="4" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="B14" s="3" t="s">
         <v>0</v>
@@ -3165,7 +3165,7 @@
     </row>
     <row r="15" spans="1:7">
       <c r="A15" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="B15" s="13">
         <v>41065</v>
@@ -3181,7 +3181,7 @@
     </row>
     <row r="16" spans="1:7">
       <c r="A16" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="B16" s="13">
         <v>41078</v>
@@ -3206,7 +3206,7 @@
     </row>
     <row r="17" spans="1:7">
       <c r="A17" s="7" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="B17" s="13">
         <v>41092</v>
@@ -3231,7 +3231,7 @@
     </row>
     <row r="18" spans="1:7">
       <c r="A18" s="7" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="B18" s="13">
         <v>41106</v>
@@ -3256,7 +3256,7 @@
     </row>
     <row r="19" spans="1:7">
       <c r="A19" s="7" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="B19" s="13">
         <v>41120</v>
@@ -3289,20 +3289,20 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.6"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13"/>
   <cols>
-    <col min="1" max="1" width="10.81640625" style="2"/>
-    <col min="2" max="2" width="24.453125" customWidth="1"/>
-    <col min="3" max="3" width="17.81640625" customWidth="1"/>
-    <col min="4" max="4" width="11.1796875" customWidth="1"/>
-    <col min="5" max="5" width="13.6328125" customWidth="1"/>
-    <col min="6" max="6" width="12.453125" style="9" customWidth="1"/>
+    <col min="1" max="1" width="10.83203125" style="2"/>
+    <col min="2" max="2" width="24.5" customWidth="1"/>
+    <col min="3" max="3" width="17.83203125" customWidth="1"/>
+    <col min="4" max="4" width="11.1640625" customWidth="1"/>
+    <col min="5" max="5" width="13.6640625" customWidth="1"/>
+    <col min="6" max="6" width="12.5" style="9" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" s="4" customFormat="1">
@@ -3398,6 +3398,27 @@
       <c r="F5" s="9">
         <f>(D5-D2)/E5*60</f>
         <v>48</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" s="2">
+        <v>42327</v>
+      </c>
+      <c r="B6">
+        <v>0</v>
+      </c>
+      <c r="C6">
+        <v>10</v>
+      </c>
+      <c r="D6">
+        <v>120</v>
+      </c>
+      <c r="E6">
+        <v>120</v>
+      </c>
+      <c r="F6" s="9">
+        <f>(D6-D2)/E6*60</f>
+        <v>60</v>
       </c>
     </row>
   </sheetData>
@@ -3416,20 +3437,20 @@
       <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.6"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13"/>
   <cols>
-    <col min="1" max="1" width="7.6328125" customWidth="1"/>
-    <col min="2" max="2" width="24.453125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="12.6328125" customWidth="1"/>
-    <col min="4" max="4" width="20.81640625" customWidth="1"/>
-    <col min="5" max="5" width="14.6328125" customWidth="1"/>
-    <col min="6" max="6" width="11.81640625" customWidth="1"/>
-    <col min="7" max="7" width="12.81640625" customWidth="1"/>
+    <col min="1" max="1" width="7.6640625" customWidth="1"/>
+    <col min="2" max="2" width="24.5" style="1" customWidth="1"/>
+    <col min="3" max="3" width="12.6640625" customWidth="1"/>
+    <col min="4" max="4" width="20.83203125" customWidth="1"/>
+    <col min="5" max="5" width="14.6640625" customWidth="1"/>
+    <col min="6" max="6" width="11.83203125" customWidth="1"/>
+    <col min="7" max="7" width="12.83203125" customWidth="1"/>
     <col min="8" max="8" width="18" customWidth="1"/>
-    <col min="9" max="9" width="10.81640625" style="6"/>
+    <col min="9" max="9" width="10.83203125" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:9" ht="14">
       <c r="A1" s="4" t="s">
         <v>9</v>
       </c>
@@ -3458,18 +3479,18 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:9" ht="14">
       <c r="A2" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="C2" s="16" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="D2" s="27" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="E2">
         <v>50</v>
@@ -3487,18 +3508,18 @@
         <v>29</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:9" ht="14">
       <c r="A3" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C3" s="16" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="D3" s="27" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="E3">
         <v>50</v>
@@ -3516,18 +3537,18 @@
         <v>29</v>
       </c>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:9" ht="14">
       <c r="A4" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C4" s="16" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="D4" s="27" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="E4">
         <v>50</v>
@@ -3545,18 +3566,18 @@
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:9" ht="14">
       <c r="A5" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C5" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="D5" s="27" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="E5">
         <v>60</v>
@@ -3574,18 +3595,18 @@
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:9" ht="14">
       <c r="A6" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="C6" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="D6" s="27" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="E6">
         <v>50</v>
@@ -3603,18 +3624,18 @@
         <v>29</v>
       </c>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:9" ht="14">
       <c r="A7" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C7" s="16" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="D7" s="27" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="E7">
         <v>70</v>
@@ -3632,18 +3653,18 @@
         <v>29</v>
       </c>
     </row>
-    <row r="8" spans="1:9">
+    <row r="8" spans="1:9" ht="14">
       <c r="A8" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C8" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="D8" s="27" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="E8">
         <v>60</v>
@@ -3661,18 +3682,18 @@
         <v>29</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="25.2">
+    <row r="9" spans="1:9" ht="28">
       <c r="A9" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="C9" s="16" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="D9" s="27" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="E9">
         <v>50</v>
@@ -3692,16 +3713,16 @@
     </row>
     <row r="10" spans="1:9">
       <c r="A10" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="B10" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C10" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="D10" s="27" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="E10">
         <v>40</v>
@@ -3721,16 +3742,16 @@
     </row>
     <row r="11" spans="1:9">
       <c r="A11" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="B11" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C11" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="D11" s="27" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="E11">
         <v>50</v>
@@ -3748,40 +3769,40 @@
         <v>29</v>
       </c>
     </row>
-    <row r="14" spans="1:9">
+    <row r="14" spans="1:9" ht="14">
       <c r="B14" s="5" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="15" spans="1:9">
+    <row r="15" spans="1:9" ht="14">
       <c r="B15" s="28" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="I15" s="7"/>
     </row>
-    <row r="16" spans="1:9">
+    <row r="16" spans="1:9" ht="14">
       <c r="B16" s="5" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="17" spans="2:2">
+    <row r="17" spans="2:2" ht="14">
       <c r="B17" s="28" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="18" spans="2:2">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="18" spans="2:2" ht="14">
       <c r="B18" s="28" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="20" spans="2:2">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="20" spans="2:2" ht="14">
       <c r="B20" s="5" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="21" spans="2:2">
+    <row r="21" spans="2:2" ht="14">
       <c r="B21" s="28" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
     </row>
   </sheetData>
@@ -3796,18 +3817,18 @@
   <dimension ref="A1:I21"/>
   <sheetViews>
     <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="E2" sqref="E2:I11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.6"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13"/>
   <cols>
-    <col min="2" max="2" width="28.1796875" customWidth="1"/>
+    <col min="2" max="2" width="28.1640625" customWidth="1"/>
     <col min="5" max="5" width="14" customWidth="1"/>
-    <col min="6" max="6" width="14.1796875" customWidth="1"/>
-    <col min="7" max="7" width="13.453125" customWidth="1"/>
+    <col min="6" max="6" width="14.1640625" customWidth="1"/>
+    <col min="7" max="7" width="13.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:9" ht="14">
       <c r="A1" s="4" t="s">
         <v>9</v>
       </c>
@@ -3838,16 +3859,16 @@
     </row>
     <row r="2" spans="1:9">
       <c r="A2" s="16" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="B2" s="17" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="C2" s="16" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="D2" s="27" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="E2">
         <v>20</v>
@@ -3862,21 +3883,21 @@
         <v>20</v>
       </c>
       <c r="I2" s="27" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
     </row>
     <row r="3" spans="1:9">
       <c r="A3" s="16" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="B3" s="17" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C3" s="16" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="D3" s="27" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="E3">
         <v>30</v>
@@ -3891,21 +3912,21 @@
         <v>20</v>
       </c>
       <c r="I3" s="27" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
     </row>
     <row r="4" spans="1:9">
       <c r="A4" s="16" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="B4" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C4" s="16" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="D4" s="27" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="E4">
         <v>30</v>
@@ -3920,21 +3941,21 @@
         <v>10</v>
       </c>
       <c r="I4" s="27" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
     </row>
     <row r="5" spans="1:9">
       <c r="A5" s="16" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="B5" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="C5" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="D5" s="27" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="E5">
         <v>20</v>
@@ -3949,21 +3970,21 @@
         <v>15</v>
       </c>
       <c r="I5" s="27" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
     </row>
     <row r="6" spans="1:9">
       <c r="A6" s="16" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="B6" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C6" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="D6" s="27" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="E6">
         <v>30</v>
@@ -3978,21 +3999,21 @@
         <v>20</v>
       </c>
       <c r="I6" s="27" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
     </row>
     <row r="7" spans="1:9">
       <c r="A7" s="16" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="B7" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C7" s="16" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="D7" s="27" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="E7">
         <v>20</v>
@@ -4007,21 +4028,21 @@
         <v>15</v>
       </c>
       <c r="I7" s="27" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
     </row>
     <row r="8" spans="1:9">
       <c r="A8" s="16" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="B8" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C8" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="D8" s="27" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="E8">
         <v>30</v>
@@ -4036,21 +4057,21 @@
         <v>20</v>
       </c>
       <c r="I8" s="27" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
     </row>
     <row r="9" spans="1:9">
       <c r="A9" s="16" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="B9" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C9" s="16" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="D9" s="27" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="E9">
         <v>30</v>
@@ -4065,21 +4086,21 @@
         <v>10</v>
       </c>
       <c r="I9" s="27" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
     </row>
     <row r="10" spans="1:9">
       <c r="A10" s="16" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="B10" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C10" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="D10" s="27" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="E10">
         <v>20</v>
@@ -4094,21 +4115,21 @@
         <v>10</v>
       </c>
       <c r="I10" s="27" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
     </row>
     <row r="11" spans="1:9">
       <c r="A11" s="16" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="B11" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C11" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="D11" s="27" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="E11">
         <v>20</v>
@@ -4123,45 +4144,45 @@
         <v>10</v>
       </c>
       <c r="I11" s="27" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="14">
       <c r="B14" s="5" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="15" spans="1:9">
+    <row r="15" spans="1:9" ht="14">
       <c r="B15" s="28" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="14">
       <c r="B16" s="5" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="17" spans="2:2">
+    <row r="17" spans="2:2" ht="14">
       <c r="B17" s="28" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="18" spans="2:2">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="18" spans="2:2" ht="14">
       <c r="B18" s="28" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
     </row>
     <row r="19" spans="2:2">
       <c r="B19" s="1"/>
     </row>
-    <row r="20" spans="2:2">
+    <row r="20" spans="2:2" ht="14">
       <c r="B20" s="5" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="21" spans="2:2">
+    <row r="21" spans="2:2" ht="14">
       <c r="B21" s="28" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
     </row>
   </sheetData>
@@ -4175,16 +4196,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:I21"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" zoomScale="150" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+    <sheetView zoomScale="150" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17:B21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.6"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13"/>
   <cols>
-    <col min="2" max="2" width="38.08984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:9" ht="14">
       <c r="A1" s="4" t="s">
         <v>3</v>
       </c>
@@ -4215,16 +4236,16 @@
     </row>
     <row r="2" spans="1:9">
       <c r="A2" s="16" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="B2" s="17" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C2" s="16" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="D2" s="27" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="E2">
         <v>20</v>
@@ -4239,21 +4260,21 @@
         <v>20</v>
       </c>
       <c r="I2" s="27" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
     </row>
     <row r="3" spans="1:9">
       <c r="A3" s="16" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="B3" s="19" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="C3" s="16" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="D3" s="27" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="E3">
         <v>30</v>
@@ -4268,21 +4289,21 @@
         <v>20</v>
       </c>
       <c r="I3" s="27" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
     </row>
     <row r="4" spans="1:9">
       <c r="A4" s="16" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="B4" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C4" s="16" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="D4" s="27" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="E4">
         <v>30</v>
@@ -4297,21 +4318,21 @@
         <v>10</v>
       </c>
       <c r="I4" s="27" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
     </row>
     <row r="5" spans="1:9">
       <c r="A5" s="16" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="B5" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="C5" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="D5" s="27" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="E5">
         <v>20</v>
@@ -4326,21 +4347,21 @@
         <v>15</v>
       </c>
       <c r="I5" s="27" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
     </row>
     <row r="6" spans="1:9">
       <c r="A6" s="16" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="B6" t="s">
-        <v>219</v>
+        <v>92</v>
       </c>
       <c r="C6" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="D6" s="27" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="E6">
         <v>30</v>
@@ -4355,21 +4376,21 @@
         <v>20</v>
       </c>
       <c r="I6" s="27" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
     </row>
     <row r="7" spans="1:9">
       <c r="A7" s="16" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="B7" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="C7" s="16" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="D7" s="27" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="E7">
         <v>20</v>
@@ -4384,21 +4405,21 @@
         <v>15</v>
       </c>
       <c r="I7" s="27" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
     </row>
     <row r="8" spans="1:9">
       <c r="A8" s="16" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="B8" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="C8" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="D8" s="27" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="E8">
         <v>30</v>
@@ -4413,21 +4434,21 @@
         <v>20</v>
       </c>
       <c r="I8" s="27" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
     </row>
     <row r="9" spans="1:9">
       <c r="A9" s="16" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="B9" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="C9" s="16" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="D9" s="27" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="E9">
         <v>30</v>
@@ -4442,21 +4463,21 @@
         <v>10</v>
       </c>
       <c r="I9" s="27" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
     </row>
     <row r="10" spans="1:9">
       <c r="A10" s="16" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="B10" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="C10" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="D10" s="27" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="E10">
         <v>20</v>
@@ -4471,21 +4492,21 @@
         <v>10</v>
       </c>
       <c r="I10" s="27" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
     </row>
     <row r="11" spans="1:9">
       <c r="A11" s="16" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="B11" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="C11" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="D11" s="27" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="E11">
         <v>20</v>
@@ -4500,45 +4521,45 @@
         <v>10</v>
       </c>
       <c r="I11" s="27" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="14">
       <c r="B14" s="5" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="15" spans="1:9">
+    <row r="15" spans="1:9" ht="14">
       <c r="B15" s="28" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="14">
       <c r="B16" s="5" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="17" spans="2:2">
+    <row r="17" spans="2:2" ht="14">
       <c r="B17" s="28" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="18" spans="2:2">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="18" spans="2:2" ht="14">
       <c r="B18" s="28" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
     </row>
     <row r="19" spans="2:2">
       <c r="B19" s="1"/>
     </row>
-    <row r="20" spans="2:2">
+    <row r="20" spans="2:2" ht="14">
       <c r="B20" s="5" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="21" spans="2:2">
+    <row r="21" spans="2:2" ht="14">
       <c r="B21" s="28" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
     </row>
   </sheetData>
@@ -4552,15 +4573,15 @@
   <dimension ref="A1:I20"/>
   <sheetViews>
     <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.6"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13"/>
   <cols>
-    <col min="2" max="2" width="28.81640625" customWidth="1"/>
+    <col min="2" max="2" width="28.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:9" ht="14">
       <c r="A1" s="4" t="s">
         <v>3</v>
       </c>
@@ -4591,36 +4612,45 @@
     </row>
     <row r="2" spans="1:9">
       <c r="A2" s="16" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="B2" s="17" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="C2" s="16" t="s">
-        <v>173</v>
-      </c>
-      <c r="D2" s="27" t="s">
-        <v>218</v>
+        <v>175</v>
+      </c>
+      <c r="D2" s="16" t="s">
+        <v>29</v>
       </c>
       <c r="E2">
         <v>20</v>
       </c>
       <c r="F2">
         <v>20</v>
+      </c>
+      <c r="G2">
+        <v>12</v>
+      </c>
+      <c r="H2">
+        <v>15</v>
+      </c>
+      <c r="I2" s="16" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:9">
       <c r="A3" s="16" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="B3" s="17" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="C3" s="16" t="s">
-        <v>169</v>
-      </c>
-      <c r="D3" s="27" t="s">
-        <v>218</v>
+        <v>171</v>
+      </c>
+      <c r="D3" s="16" t="s">
+        <v>29</v>
       </c>
       <c r="E3">
         <v>30</v>
@@ -4628,19 +4658,28 @@
       <c r="F3">
         <v>30</v>
       </c>
+      <c r="G3">
+        <v>11</v>
+      </c>
+      <c r="H3">
+        <v>15</v>
+      </c>
+      <c r="I3" s="16" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="4" spans="1:9">
       <c r="A4" s="16" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="B4" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="C4" s="16" t="s">
-        <v>170</v>
-      </c>
-      <c r="D4" s="27" t="s">
-        <v>218</v>
+        <v>172</v>
+      </c>
+      <c r="D4" s="16" t="s">
+        <v>29</v>
       </c>
       <c r="E4">
         <v>30</v>
@@ -4648,19 +4687,28 @@
       <c r="F4">
         <v>30</v>
       </c>
+      <c r="G4">
+        <v>12</v>
+      </c>
+      <c r="H4">
+        <v>10</v>
+      </c>
+      <c r="I4" s="16" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="5" spans="1:9">
       <c r="A5" s="16" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="B5" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="C5" t="s">
-        <v>170</v>
-      </c>
-      <c r="D5" s="27" t="s">
-        <v>218</v>
+        <v>172</v>
+      </c>
+      <c r="D5" s="16" t="s">
+        <v>29</v>
       </c>
       <c r="E5">
         <v>20</v>
@@ -4668,19 +4716,28 @@
       <c r="F5">
         <v>30</v>
       </c>
+      <c r="G5">
+        <v>12</v>
+      </c>
+      <c r="H5">
+        <v>15</v>
+      </c>
+      <c r="I5" s="16" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="6" spans="1:9">
       <c r="A6" s="16" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="B6" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="C6" t="s">
-        <v>171</v>
-      </c>
-      <c r="D6" s="27" t="s">
-        <v>218</v>
+        <v>173</v>
+      </c>
+      <c r="D6" s="16" t="s">
+        <v>29</v>
       </c>
       <c r="E6">
         <v>30</v>
@@ -4688,39 +4745,57 @@
       <c r="F6">
         <v>30</v>
       </c>
+      <c r="G6">
+        <v>10</v>
+      </c>
+      <c r="H6">
+        <v>20</v>
+      </c>
+      <c r="I6" s="16" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="7" spans="1:9">
       <c r="A7" s="16" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="B7" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="C7" s="16" t="s">
-        <v>174</v>
-      </c>
-      <c r="D7" s="27" t="s">
-        <v>218</v>
+        <v>176</v>
+      </c>
+      <c r="D7" s="16" t="s">
+        <v>29</v>
       </c>
       <c r="E7">
         <v>20</v>
       </c>
       <c r="F7">
         <v>20</v>
+      </c>
+      <c r="G7">
+        <v>12</v>
+      </c>
+      <c r="H7">
+        <v>15</v>
+      </c>
+      <c r="I7" s="16" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="8" spans="1:9">
       <c r="A8" s="16" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="B8" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="C8" t="s">
-        <v>168</v>
-      </c>
-      <c r="D8" s="27" t="s">
-        <v>218</v>
+        <v>170</v>
+      </c>
+      <c r="D8" s="16" t="s">
+        <v>29</v>
       </c>
       <c r="E8">
         <v>30</v>
@@ -4728,19 +4803,28 @@
       <c r="F8">
         <v>20</v>
       </c>
+      <c r="G8">
+        <v>12</v>
+      </c>
+      <c r="H8">
+        <v>20</v>
+      </c>
+      <c r="I8" s="16" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="9" spans="1:9">
       <c r="A9" s="16" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="B9" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="C9" s="16" t="s">
-        <v>175</v>
-      </c>
-      <c r="D9" s="27" t="s">
-        <v>218</v>
+        <v>177</v>
+      </c>
+      <c r="D9" s="16" t="s">
+        <v>29</v>
       </c>
       <c r="E9">
         <v>30</v>
@@ -4748,39 +4832,57 @@
       <c r="F9">
         <v>20</v>
       </c>
+      <c r="G9">
+        <v>15</v>
+      </c>
+      <c r="H9">
+        <v>10</v>
+      </c>
+      <c r="I9" s="16" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="10" spans="1:9">
       <c r="A10" s="16" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="B10" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="C10" t="s">
-        <v>172</v>
-      </c>
-      <c r="D10" s="27" t="s">
-        <v>218</v>
+        <v>174</v>
+      </c>
+      <c r="D10" s="16" t="s">
+        <v>29</v>
       </c>
       <c r="E10">
         <v>20</v>
       </c>
       <c r="F10">
         <v>20</v>
+      </c>
+      <c r="G10">
+        <v>13</v>
+      </c>
+      <c r="H10">
+        <v>10</v>
+      </c>
+      <c r="I10" s="16" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="11" spans="1:9">
       <c r="A11" s="16" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="B11" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="C11" t="s">
-        <v>172</v>
-      </c>
-      <c r="D11" s="27" t="s">
-        <v>218</v>
+        <v>174</v>
+      </c>
+      <c r="D11" s="16" t="s">
+        <v>29</v>
       </c>
       <c r="E11">
         <v>20</v>
@@ -4788,36 +4890,53 @@
       <c r="F11">
         <v>20</v>
       </c>
-    </row>
-    <row r="13" spans="1:9">
+      <c r="G11">
+        <v>11</v>
+      </c>
+      <c r="H11">
+        <v>10</v>
+      </c>
+      <c r="I11" s="16" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="14">
       <c r="B13" s="5" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="14" spans="1:9">
-      <c r="B14" s="28"/>
-    </row>
-    <row r="15" spans="1:9">
+    <row r="14" spans="1:9" ht="14">
+      <c r="B14" s="28" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="14">
       <c r="B15" s="5" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="16" spans="1:9">
-      <c r="B16" s="28"/>
-    </row>
-    <row r="17" spans="2:2">
-      <c r="B17" s="28"/>
+    <row r="16" spans="1:9" ht="14">
+      <c r="B16" s="28" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="17" spans="2:2" ht="14">
+      <c r="B17" s="28" t="s">
+        <v>209</v>
+      </c>
     </row>
     <row r="18" spans="2:2">
       <c r="B18" s="1"/>
     </row>
-    <row r="19" spans="2:2">
+    <row r="19" spans="2:2" ht="14">
       <c r="B19" s="5" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="20" spans="2:2">
-      <c r="B20" s="28"/>
+    <row r="20" spans="2:2" ht="14">
+      <c r="B20" s="28" t="s">
+        <v>210</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
@@ -4829,471 +4948,471 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:C43"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" zoomScale="118" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+    <sheetView topLeftCell="A28" zoomScale="118" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="G39" sqref="G39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.6"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13"/>
   <cols>
-    <col min="2" max="2" width="37.54296875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="68.453125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="28.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="68.5" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="4" customFormat="1">
+    <row r="1" spans="1:3" s="4" customFormat="1" ht="14">
       <c r="A1" s="4" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="15">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="17">
       <c r="A2" s="17" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="B2" s="17" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="C2" s="18" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="15">
+    <row r="3" spans="1:3" ht="17">
       <c r="A3" s="17" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="B3" s="17" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C3" s="18" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="15">
+    <row r="4" spans="1:3" ht="17">
       <c r="A4" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="B4" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C4" s="12" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="30">
+    <row r="5" spans="1:3" ht="34">
       <c r="A5" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="B5" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C5" s="12" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="15">
+    <row r="6" spans="1:3" ht="17">
       <c r="A6" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="B6" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="C6" s="12" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="15">
+    <row r="7" spans="1:3" ht="17">
       <c r="A7" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="B7" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C7" s="12" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="30">
+    <row r="8" spans="1:3" ht="34">
       <c r="A8" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="B8" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C8" s="12" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" ht="30">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="34">
       <c r="A9" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="B9" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="C9" s="12" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" ht="30">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="34">
       <c r="A10" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="B10" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C10" s="12" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" ht="30">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="34">
       <c r="A11" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="B11" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C11" s="12" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" ht="15">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="17">
       <c r="A12" s="17" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="B12" s="17" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="C12" s="18" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="30">
+    <row r="13" spans="1:3" ht="34">
       <c r="A13" s="17" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="B13" s="17" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C13" s="18" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" ht="45">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="51">
       <c r="A14" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="B14" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C14" s="12" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" ht="15">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="17">
       <c r="A15" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="B15" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="C15" s="12" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="15">
+    <row r="16" spans="1:3" ht="17">
       <c r="A16" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="B16" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C16" s="12" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="15">
+    <row r="17" spans="1:3" ht="17">
       <c r="A17" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="B17" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C17" s="12" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="15">
+    <row r="18" spans="1:3" ht="17">
       <c r="A18" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="B18" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C18" s="12" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="15">
+    <row r="19" spans="1:3" ht="17">
       <c r="A19" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="B19" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C19" s="12" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="15">
+    <row r="20" spans="1:3" ht="17">
       <c r="A20" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="B20" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C20" s="12" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="15">
+    <row r="21" spans="1:3" ht="17">
       <c r="A21" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="B21" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C21" s="12" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="15">
+    <row r="22" spans="1:3" ht="17">
       <c r="A22" s="17" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="B22" s="17" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C22" s="18" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" ht="15">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="17">
       <c r="A23" s="17" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="B23" s="19" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="C23" s="18" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" ht="30">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="34">
       <c r="A24" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="B24" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C24" s="12" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="30">
+    <row r="25" spans="1:3" ht="34">
       <c r="A25" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="B25" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="C25" s="12" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="15">
+    <row r="26" spans="1:3" ht="34">
       <c r="A26" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="B26" t="s">
+        <v>92</v>
+      </c>
+      <c r="C26" s="12" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" ht="85">
+      <c r="A27" t="s">
+        <v>135</v>
+      </c>
+      <c r="B27" t="s">
+        <v>93</v>
+      </c>
+      <c r="C27" s="12" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" ht="17">
+      <c r="A28" t="s">
+        <v>136</v>
+      </c>
+      <c r="B28" t="s">
+        <v>94</v>
+      </c>
+      <c r="C28" s="12" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" ht="17">
+      <c r="A29" t="s">
+        <v>137</v>
+      </c>
+      <c r="B29" t="s">
+        <v>95</v>
+      </c>
+      <c r="C29" s="12" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" ht="17">
+      <c r="A30" t="s">
+        <v>138</v>
+      </c>
+      <c r="B30" t="s">
+        <v>96</v>
+      </c>
+      <c r="C30" s="12" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" ht="17">
+      <c r="A31" t="s">
+        <v>139</v>
+      </c>
+      <c r="B31" t="s">
+        <v>97</v>
+      </c>
+      <c r="C31" s="12" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" ht="34">
+      <c r="A32" s="17" t="s">
+        <v>140</v>
+      </c>
+      <c r="B32" s="19" t="s">
         <v>219</v>
       </c>
-      <c r="C26" s="12" t="s">
+      <c r="C32" s="18" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" ht="17">
+      <c r="A33" s="17" t="s">
+        <v>141</v>
+      </c>
+      <c r="B33" s="19" t="s">
         <v>220</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" ht="75">
-      <c r="A27" t="s">
-        <v>133</v>
-      </c>
-      <c r="B27" t="s">
-        <v>91</v>
-      </c>
-      <c r="C27" s="12" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" ht="15">
-      <c r="A28" t="s">
-        <v>134</v>
-      </c>
-      <c r="B28" t="s">
-        <v>92</v>
-      </c>
-      <c r="C28" s="12" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" ht="15">
-      <c r="A29" t="s">
-        <v>135</v>
-      </c>
-      <c r="B29" t="s">
-        <v>93</v>
-      </c>
-      <c r="C29" s="12" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" ht="15">
-      <c r="A30" t="s">
-        <v>136</v>
-      </c>
-      <c r="B30" t="s">
-        <v>94</v>
-      </c>
-      <c r="C30" s="12" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" ht="15">
-      <c r="A31" t="s">
-        <v>137</v>
-      </c>
-      <c r="B31" t="s">
-        <v>95</v>
-      </c>
-      <c r="C31" s="12" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" ht="15">
-      <c r="A32" s="17" t="s">
-        <v>138</v>
-      </c>
-      <c r="B32" s="17" t="s">
-        <v>96</v>
-      </c>
-      <c r="C32" s="18" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" ht="15">
-      <c r="A33" s="17" t="s">
-        <v>139</v>
-      </c>
-      <c r="B33" s="17" t="s">
-        <v>97</v>
-      </c>
       <c r="C33" s="18" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" ht="30">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" ht="34">
       <c r="A34" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="B34" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="C34" s="12" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" ht="30">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" ht="34">
       <c r="A35" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="B35" t="s">
+        <v>108</v>
+      </c>
+      <c r="C35" s="12" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" ht="17">
+      <c r="A36" t="s">
+        <v>144</v>
+      </c>
+      <c r="B36" t="s">
+        <v>101</v>
+      </c>
+      <c r="C36" s="12" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" ht="17">
+      <c r="A37" t="s">
+        <v>145</v>
+      </c>
+      <c r="B37" t="s">
+        <v>102</v>
+      </c>
+      <c r="C37" s="12" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" ht="34">
+      <c r="A38" t="s">
+        <v>146</v>
+      </c>
+      <c r="B38" t="s">
+        <v>103</v>
+      </c>
+      <c r="C38" s="12" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" ht="34">
+      <c r="A39" t="s">
+        <v>147</v>
+      </c>
+      <c r="B39" t="s">
+        <v>104</v>
+      </c>
+      <c r="C39" s="12" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" ht="34">
+      <c r="A40" t="s">
+        <v>148</v>
+      </c>
+      <c r="B40" t="s">
+        <v>105</v>
+      </c>
+      <c r="C40" s="12" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" ht="17">
+      <c r="A41" t="s">
+        <v>149</v>
+      </c>
+      <c r="B41" t="s">
         <v>106</v>
       </c>
-      <c r="C35" s="12" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" ht="15">
-      <c r="A36" t="s">
-        <v>142</v>
-      </c>
-      <c r="B36" t="s">
-        <v>99</v>
-      </c>
-      <c r="C36" s="12" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" ht="15">
-      <c r="A37" t="s">
-        <v>143</v>
-      </c>
-      <c r="B37" t="s">
-        <v>100</v>
-      </c>
-      <c r="C37" s="12" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" ht="30">
-      <c r="A38" t="s">
-        <v>144</v>
-      </c>
-      <c r="B38" t="s">
-        <v>101</v>
-      </c>
-      <c r="C38" s="12" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" ht="15">
-      <c r="A39" t="s">
-        <v>145</v>
-      </c>
-      <c r="B39" t="s">
-        <v>102</v>
-      </c>
-      <c r="C39" s="12" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" ht="30">
-      <c r="A40" t="s">
-        <v>146</v>
-      </c>
-      <c r="B40" t="s">
-        <v>103</v>
-      </c>
-      <c r="C40" s="12" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" ht="15">
-      <c r="A41" t="s">
-        <v>147</v>
-      </c>
-      <c r="B41" t="s">
-        <v>104</v>
-      </c>
       <c r="C41" s="12" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" ht="15">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" ht="16">
       <c r="C42" s="12"/>
     </row>
-    <row r="43" spans="1:3" ht="15">
+    <row r="43" spans="1:3" ht="16">
       <c r="C43" s="12"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Modified Descriptions of a few User Stories
</commit_message>
<xml_diff>
--- a/Team05Report.xlsx
+++ b/Team05Report.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22130"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vctu\OneDrive\Code\Python\2019fall-Group5-555B-Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\samar\Downloads\Scanned pics\New\Assignments\Agile\Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3" documentId="13_ncr:1_{11BD8F8C-6159-894E-820F-70B181C205AD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{04C8A05C-C889-41A5-9EB0-9AC85E34A1C8}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFEB12E9-2DA6-407E-AD74-4538F103369C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1310" yWindow="3570" windowWidth="28800" windowHeight="15460" tabRatio="500" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" firstSheet="2" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="610" uniqueCount="225">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="610" uniqueCount="228">
   <si>
     <t>Date</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -231,9 +231,6 @@
     <t>No more than one family with the same spouses by name and the same marriage date should appear in a GEDCOM file</t>
   </si>
   <si>
-    <t>No more than one child with the same name and birth date should appear in a family</t>
-  </si>
-  <si>
     <t>Include person's current age when listing individuals</t>
   </si>
   <si>
@@ -571,9 +568,6 @@
   </si>
   <si>
     <t>Birth dates of siblings should be more than 8 months apart or less than 2 days apart (twins may be born one day apart, e.g. 11:59 PM and 12:02 AM the following calendar day)</t>
-  </si>
-  <si>
-    <t>All family roles (spouse, child) specified in an individual record should have corresponding entries in the corresponding family records. Likewise, all individual roles (spouse, child) specified in family records should have corresponding entries in the corresponding  individual's records.  I.e. the information in the individual and family records should be consistent.</t>
   </si>
   <si>
     <t>List siblings in families by decreasing age, i.e. oldest siblings first</t>
@@ -831,16 +825,31 @@
     <t>List large age differences</t>
     <phoneticPr fontId="6" type="noConversion"/>
   </si>
+  <si>
+    <t>Unique first names of childs in families</t>
+  </si>
+  <si>
+    <t>No more than one child with the same name should appear in a family</t>
+  </si>
+  <si>
+    <t>List All births</t>
+  </si>
+  <si>
+    <t>Liat All births</t>
+  </si>
+  <si>
+    <t>List all the birthdays in the GEDCOM File</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="176" formatCode="m/d"/>
-    <numFmt numFmtId="177" formatCode="0.0"/>
+    <numFmt numFmtId="164" formatCode="m/d"/>
+    <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="13">
     <font>
       <sz val="10"/>
       <name val="Verdana"/>
@@ -1016,20 +1025,20 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="176" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="177" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="176" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -1037,7 +1046,7 @@
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="177" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1050,79 +1059,79 @@
     <xf numFmtId="49" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="65" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="176" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="66">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
-    <cellStyle name="超链接" xfId="1" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="3" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="5" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="7" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="9" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="11" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="13" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="15" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="17" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="19" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="21" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="23" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="25" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="27" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="29" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="31" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="33" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="35" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="37" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="39" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="41" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="43" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="45" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="47" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="49" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="51" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="53" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="55" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="57" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="59" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="61" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="63" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="65" builtinId="8"/>
-    <cellStyle name="已访问的超链接" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="4" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="6" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="8" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="10" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="12" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="14" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="16" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="18" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="20" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="22" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="24" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="26" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="28" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="30" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="32" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="34" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="36" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="38" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="40" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="42" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="44" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="46" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="48" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="50" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="52" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="54" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="56" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="58" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="60" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="62" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="64" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="64" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="59" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="61" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="63" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="65" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
@@ -1140,7 +1149,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="1"/>
-  <c:lang val="zh-CN"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1277,7 +1286,7 @@
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="1"/>
-  <c:lang val="zh-CN"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -2234,15 +2243,15 @@
       <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.6"/>
   <cols>
-    <col min="1" max="1" width="7.84375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.81640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18" customWidth="1"/>
-    <col min="3" max="3" width="8.4609375" customWidth="1"/>
-    <col min="4" max="5" width="20.4609375" customWidth="1"/>
+    <col min="3" max="3" width="8.453125" customWidth="1"/>
+    <col min="4" max="5" width="20.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" s="4" customFormat="1">
       <c r="A1" s="4" t="s">
         <v>19</v>
       </c>
@@ -2259,110 +2268,110 @@
         <v>34</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7">
       <c r="A2" s="20" t="s">
+        <v>175</v>
+      </c>
+      <c r="B2" s="20" t="s">
+        <v>176</v>
+      </c>
+      <c r="C2" s="20" t="s">
         <v>177</v>
       </c>
-      <c r="B2" s="20" t="s">
+      <c r="D2" s="21" t="s">
+        <v>191</v>
+      </c>
+      <c r="E2" s="20" t="s">
         <v>178</v>
       </c>
-      <c r="C2" s="20" t="s">
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" s="20" t="s">
+        <v>169</v>
+      </c>
+      <c r="B3" s="20" t="s">
         <v>179</v>
       </c>
-      <c r="D2" s="21" t="s">
+      <c r="C3" s="20" t="s">
+        <v>180</v>
+      </c>
+      <c r="D3" s="21" t="s">
+        <v>192</v>
+      </c>
+      <c r="E3" s="20" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" s="20" t="s">
+        <v>170</v>
+      </c>
+      <c r="B4" s="20" t="s">
+        <v>182</v>
+      </c>
+      <c r="C4" s="20" t="s">
+        <v>183</v>
+      </c>
+      <c r="D4" s="21" t="s">
         <v>193</v>
       </c>
-      <c r="E2" s="20" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3" s="20" t="s">
-        <v>171</v>
-      </c>
-      <c r="B3" s="20" t="s">
-        <v>181</v>
-      </c>
-      <c r="C3" s="20" t="s">
-        <v>182</v>
-      </c>
-      <c r="D3" s="21" t="s">
+      <c r="E4" s="20" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5" s="20" t="s">
+        <v>168</v>
+      </c>
+      <c r="B5" s="20" t="s">
+        <v>185</v>
+      </c>
+      <c r="C5" s="20" t="s">
+        <v>186</v>
+      </c>
+      <c r="D5" s="21" t="s">
         <v>194</v>
       </c>
-      <c r="E3" s="20" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A4" s="20" t="s">
-        <v>172</v>
-      </c>
-      <c r="B4" s="20" t="s">
-        <v>184</v>
-      </c>
-      <c r="C4" s="20" t="s">
-        <v>185</v>
-      </c>
-      <c r="D4" s="21" t="s">
+      <c r="E5" s="20" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6" s="20" t="s">
+        <v>166</v>
+      </c>
+      <c r="B6" s="20" t="s">
+        <v>188</v>
+      </c>
+      <c r="C6" s="20" t="s">
+        <v>189</v>
+      </c>
+      <c r="D6" s="21" t="s">
         <v>195</v>
       </c>
-      <c r="E4" s="20" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A5" s="20" t="s">
-        <v>170</v>
-      </c>
-      <c r="B5" s="20" t="s">
-        <v>187</v>
-      </c>
-      <c r="C5" s="20" t="s">
-        <v>188</v>
-      </c>
-      <c r="D5" s="21" t="s">
-        <v>196</v>
-      </c>
-      <c r="E5" s="20" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A6" s="20" t="s">
-        <v>168</v>
-      </c>
-      <c r="B6" s="20" t="s">
+      <c r="E6" s="20" t="s">
         <v>190</v>
       </c>
-      <c r="C6" s="20" t="s">
-        <v>191</v>
-      </c>
-      <c r="D6" s="21" t="s">
-        <v>197</v>
-      </c>
-      <c r="E6" s="20" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="7" spans="1:7">
       <c r="D7" s="22"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7">
       <c r="D9" s="23" t="s">
         <v>35</v>
       </c>
       <c r="E9" s="21" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="F9" s="24"/>
       <c r="G9" s="24"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7">
       <c r="D10" s="24" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="E10" s="25" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="F10" s="24"/>
       <c r="G10" s="24"/>
@@ -2393,16 +2402,16 @@
       <selection activeCell="C41" sqref="C41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.6"/>
   <cols>
-    <col min="1" max="1" width="5.15234375" customWidth="1"/>
-    <col min="2" max="2" width="9.69140625" customWidth="1"/>
+    <col min="1" max="1" width="5.1796875" customWidth="1"/>
+    <col min="2" max="2" width="9.7265625" customWidth="1"/>
     <col min="3" max="3" width="31" customWidth="1"/>
-    <col min="4" max="4" width="6.69140625" customWidth="1"/>
-    <col min="5" max="5" width="7.69140625" customWidth="1"/>
+    <col min="4" max="4" width="6.7265625" customWidth="1"/>
+    <col min="5" max="5" width="7.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" s="4" customFormat="1">
       <c r="A1" s="4" t="s">
         <v>30</v>
       </c>
@@ -2419,684 +2428,684 @@
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" s="16" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="C2" s="17" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D2" s="16" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="E2" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" s="16" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="C3" s="17" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D3" s="16" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="E3" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" s="16" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="C4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D4" s="16" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="E4" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" s="16" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D5" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="E5" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" s="16" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C6" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D6" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="E6" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" s="16" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C7" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D7" s="16" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="E7" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" s="16" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C8" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D8" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="E8" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9" s="16" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C9" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D9" s="16" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="E9" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10" s="16" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C10" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D10" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="E10" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11" s="16" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C11" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D11" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="E11" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5">
       <c r="A12">
         <v>11</v>
       </c>
       <c r="B12" s="16" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C12" s="17" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D12" s="16" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="E12" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5">
       <c r="A13">
         <v>12</v>
       </c>
       <c r="B13" s="16" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C13" s="17" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D13" s="16" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="E13" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5">
       <c r="A14">
         <v>13</v>
       </c>
       <c r="B14" s="16" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C14" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D14" s="16" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="E14" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5">
       <c r="A15">
         <v>14</v>
       </c>
       <c r="B15" s="16" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C15" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D15" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="E15" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5">
       <c r="A16">
         <v>15</v>
       </c>
       <c r="B16" s="16" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C16" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D16" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="E16" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5">
       <c r="A17">
         <v>16</v>
       </c>
       <c r="B17" s="16" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C17" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D17" s="16" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="E17" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5">
       <c r="A18">
         <v>17</v>
       </c>
       <c r="B18" s="16" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C18" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D18" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="E18" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5">
       <c r="A19">
         <v>18</v>
       </c>
       <c r="B19" s="16" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C19" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D19" s="16" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="E19" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5">
       <c r="A20">
         <v>19</v>
       </c>
       <c r="B20" s="16" t="s">
+        <v>125</v>
+      </c>
+      <c r="C20" t="s">
+        <v>84</v>
+      </c>
+      <c r="D20" t="s">
+        <v>170</v>
+      </c>
+      <c r="E20" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21" s="16" t="s">
         <v>126</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C21" t="s">
         <v>85</v>
       </c>
-      <c r="D20" t="s">
-        <v>172</v>
-      </c>
-      <c r="E20" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A21">
-        <v>20</v>
-      </c>
-      <c r="B21" s="16" t="s">
-        <v>127</v>
-      </c>
-      <c r="C21" t="s">
-        <v>86</v>
-      </c>
       <c r="D21" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="E21" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5">
       <c r="A22">
         <v>21</v>
       </c>
       <c r="B22" s="16" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C22" s="17" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D22" s="16" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="E22" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5">
       <c r="A23">
         <v>22</v>
       </c>
       <c r="B23" s="16" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C23" s="19" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="D23" s="16" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="E23" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5">
       <c r="A24">
         <v>23</v>
       </c>
       <c r="B24" s="16" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C24" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D24" s="16" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="E24" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:5">
       <c r="A25">
         <v>24</v>
       </c>
       <c r="B25" s="16" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C25" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D25" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="E25" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:5">
       <c r="A26">
         <v>25</v>
       </c>
       <c r="B26" s="16" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C26" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D26" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="E26" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:5">
       <c r="A27">
         <v>26</v>
       </c>
       <c r="B27" s="16" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C27" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D27" s="16" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="E27" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:5">
       <c r="A28">
         <v>27</v>
       </c>
       <c r="B28" s="16" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C28" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D28" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="E28" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:5">
       <c r="A29">
         <v>28</v>
       </c>
       <c r="B29" s="16" t="s">
+        <v>134</v>
+      </c>
+      <c r="C29" t="s">
+        <v>94</v>
+      </c>
+      <c r="D29" s="16" t="s">
+        <v>173</v>
+      </c>
+      <c r="E29" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5">
+      <c r="A30">
+        <v>29</v>
+      </c>
+      <c r="B30" s="16" t="s">
         <v>135</v>
       </c>
-      <c r="C29" t="s">
+      <c r="C30" t="s">
         <v>95</v>
       </c>
-      <c r="D29" s="16" t="s">
-        <v>175</v>
-      </c>
-      <c r="E29" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A30">
-        <v>29</v>
-      </c>
-      <c r="B30" s="16" t="s">
-        <v>136</v>
-      </c>
-      <c r="C30" t="s">
-        <v>96</v>
-      </c>
       <c r="D30" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="E30" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:5">
       <c r="A31">
         <v>30</v>
       </c>
       <c r="B31" s="16" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C31" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D31" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="E31" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:5">
       <c r="A32">
         <v>31</v>
       </c>
       <c r="B32" s="16" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C32" s="17" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D32" s="16" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="E32" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:5">
       <c r="A33">
         <v>32</v>
       </c>
       <c r="B33" s="16" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C33" s="17" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D33" s="16" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="E33" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:5">
       <c r="A34">
         <v>33</v>
       </c>
       <c r="B34" s="16" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C34" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D34" s="16" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="E34" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:5">
       <c r="A35">
         <v>34</v>
       </c>
       <c r="B35" s="16" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C35" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D35" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="E35" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:5">
       <c r="A36">
         <v>35</v>
       </c>
       <c r="B36" s="16" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C36" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D36" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="E36" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:5">
       <c r="A37">
         <v>36</v>
       </c>
       <c r="B37" s="16" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C37" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D37" s="16" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="E37" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:5">
       <c r="A38">
         <v>37</v>
       </c>
       <c r="B38" s="16" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C38" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D38" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="E38" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:5">
       <c r="A39">
         <v>38</v>
       </c>
       <c r="B39" s="16" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C39" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D39" s="16" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="E39" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:5">
       <c r="A40">
         <v>39</v>
       </c>
       <c r="B40" s="16" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C40" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D40" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="E40" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:5">
       <c r="A41">
         <v>40</v>
       </c>
       <c r="B41" s="16" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C41" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="D41" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="E41" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
   </sheetData>
@@ -3114,49 +3123,49 @@
       <selection activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.6"/>
   <cols>
-    <col min="1" max="1" width="10.84375" style="7"/>
-    <col min="2" max="2" width="9.4609375" customWidth="1"/>
-    <col min="3" max="3" width="15.84375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.3046875" customWidth="1"/>
-    <col min="5" max="5" width="6.84375" customWidth="1"/>
-    <col min="6" max="6" width="12.4609375" style="9" customWidth="1"/>
+    <col min="1" max="1" width="10.81640625" style="7"/>
+    <col min="2" max="2" width="9.453125" customWidth="1"/>
+    <col min="3" max="3" width="15.81640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.26953125" customWidth="1"/>
+    <col min="5" max="5" width="6.81640625" customWidth="1"/>
+    <col min="6" max="6" width="12.453125" style="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7">
       <c r="A1" s="7" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" s="7" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2" s="7" t="s">
+    <row r="3" spans="1:7">
+      <c r="A3" s="7" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3" s="7" t="s">
+    <row r="5" spans="1:7">
+      <c r="A5" s="7" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6" s="7" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8" s="7" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" s="4" customFormat="1">
+      <c r="A14" s="4" t="s">
         <v>152</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A5" s="7" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A6" s="7" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A8" s="7" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="4" t="s">
-        <v>153</v>
       </c>
       <c r="B14" s="3" t="s">
         <v>0</v>
@@ -3177,9 +3186,9 @@
         <v>24</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7">
       <c r="A15" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B15" s="13">
         <v>41065</v>
@@ -3193,9 +3202,9 @@
       <c r="F15" s="14"/>
       <c r="G15" s="9"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7">
       <c r="A16" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B16" s="13">
         <v>41078</v>
@@ -3218,9 +3227,9 @@
         <v>125.00000000000001</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7">
       <c r="A17" s="7" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B17" s="13">
         <v>41092</v>
@@ -3243,9 +3252,9 @@
         <v>102.22222222222223</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7">
       <c r="A18" s="7" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B18" s="13">
         <v>41106</v>
@@ -3268,9 +3277,9 @@
         <v>97.5</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:7">
       <c r="A19" s="7" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B19" s="13">
         <v>41120</v>
@@ -3309,17 +3318,17 @@
       <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.6"/>
   <cols>
-    <col min="1" max="1" width="10.84375" style="2"/>
-    <col min="2" max="2" width="24.4609375" customWidth="1"/>
-    <col min="3" max="3" width="17.84375" customWidth="1"/>
-    <col min="4" max="4" width="11.15234375" customWidth="1"/>
-    <col min="5" max="5" width="13.69140625" customWidth="1"/>
-    <col min="6" max="6" width="12.4609375" style="9" customWidth="1"/>
+    <col min="1" max="1" width="10.81640625" style="2"/>
+    <col min="2" max="2" width="24.453125" customWidth="1"/>
+    <col min="3" max="3" width="17.81640625" customWidth="1"/>
+    <col min="4" max="4" width="11.1796875" customWidth="1"/>
+    <col min="5" max="5" width="13.7265625" customWidth="1"/>
+    <col min="6" max="6" width="12.453125" style="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" s="4" customFormat="1">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -3339,7 +3348,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6">
       <c r="A2" s="2">
         <v>42271</v>
       </c>
@@ -3350,7 +3359,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6">
       <c r="A3" s="2">
         <v>42285</v>
       </c>
@@ -3372,7 +3381,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6">
       <c r="A4" s="2">
         <v>42299</v>
       </c>
@@ -3393,7 +3402,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6">
       <c r="A5" s="2">
         <v>42313</v>
       </c>
@@ -3414,7 +3423,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6">
       <c r="A6" s="2">
         <v>42327</v>
       </c>
@@ -3451,20 +3460,20 @@
       <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.6"/>
   <cols>
-    <col min="1" max="1" width="7.69140625" customWidth="1"/>
-    <col min="2" max="2" width="24.4609375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="12.69140625" customWidth="1"/>
-    <col min="4" max="4" width="20.84375" customWidth="1"/>
-    <col min="5" max="5" width="14.69140625" customWidth="1"/>
-    <col min="6" max="6" width="11.84375" customWidth="1"/>
-    <col min="7" max="7" width="12.84375" customWidth="1"/>
+    <col min="1" max="1" width="7.7265625" customWidth="1"/>
+    <col min="2" max="2" width="24.453125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="12.7265625" customWidth="1"/>
+    <col min="4" max="4" width="20.81640625" customWidth="1"/>
+    <col min="5" max="5" width="14.7265625" customWidth="1"/>
+    <col min="6" max="6" width="11.81640625" customWidth="1"/>
+    <col min="7" max="7" width="12.81640625" customWidth="1"/>
     <col min="8" max="8" width="18" customWidth="1"/>
-    <col min="9" max="9" width="10.84375" style="6"/>
+    <col min="9" max="9" width="10.81640625" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9">
       <c r="A1" s="4" t="s">
         <v>9</v>
       </c>
@@ -3493,18 +3502,18 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9">
       <c r="A2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C2" s="16" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="D2" s="27" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="E2">
         <v>50</v>
@@ -3522,18 +3531,18 @@
         <v>29</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9">
       <c r="A3" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C3" s="16" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="D3" s="27" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="E3">
         <v>50</v>
@@ -3551,18 +3560,18 @@
         <v>29</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9">
       <c r="A4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C4" s="16" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="D4" s="27" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="E4">
         <v>50</v>
@@ -3580,18 +3589,18 @@
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9">
       <c r="A5" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C5" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="D5" s="27" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="E5">
         <v>60</v>
@@ -3609,18 +3618,18 @@
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9">
       <c r="A6" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C6" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="D6" s="27" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="E6">
         <v>50</v>
@@ -3638,18 +3647,18 @@
         <v>29</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9">
       <c r="A7" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C7" s="16" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="D7" s="27" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="E7">
         <v>70</v>
@@ -3667,18 +3676,18 @@
         <v>29</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9">
       <c r="A8" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C8" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="D8" s="27" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="E8">
         <v>60</v>
@@ -3696,18 +3705,18 @@
         <v>29</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="27" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" ht="25.2">
       <c r="A9" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C9" s="16" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="D9" s="27" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="E9">
         <v>50</v>
@@ -3725,18 +3734,18 @@
         <v>29</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9">
       <c r="A10" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B10" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C10" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="D10" s="27" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="E10">
         <v>40</v>
@@ -3754,18 +3763,18 @@
         <v>29</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9">
       <c r="A11" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B11" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C11" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="D11" s="27" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="E11">
         <v>50</v>
@@ -3783,40 +3792,40 @@
         <v>29</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9">
       <c r="B14" s="5" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9">
       <c r="B15" s="28" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="I15" s="7"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9">
       <c r="B16" s="5" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:2">
       <c r="B17" s="28" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.3">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="18" spans="2:2">
       <c r="B18" s="28" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="20" spans="2:2" x14ac:dyDescent="0.3">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="20" spans="2:2">
       <c r="B20" s="5" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="21" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:2">
       <c r="B21" s="28" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
     </row>
   </sheetData>
@@ -3834,15 +3843,15 @@
       <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.6"/>
   <cols>
-    <col min="2" max="2" width="28.15234375" customWidth="1"/>
+    <col min="2" max="2" width="28.1796875" customWidth="1"/>
     <col min="5" max="5" width="14" customWidth="1"/>
-    <col min="6" max="6" width="14.15234375" customWidth="1"/>
-    <col min="7" max="7" width="13.4609375" customWidth="1"/>
+    <col min="6" max="6" width="14.1796875" customWidth="1"/>
+    <col min="7" max="7" width="13.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9">
       <c r="A1" s="4" t="s">
         <v>9</v>
       </c>
@@ -3871,18 +3880,18 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9">
       <c r="A2" s="16" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="B2" s="17" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C2" s="16" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="D2" s="27" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="E2">
         <v>20</v>
@@ -3897,21 +3906,21 @@
         <v>20</v>
       </c>
       <c r="I2" s="27" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
       <c r="A3" s="16" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="B3" s="17" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C3" s="16" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="D3" s="27" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="E3">
         <v>30</v>
@@ -3926,21 +3935,21 @@
         <v>20</v>
       </c>
       <c r="I3" s="27" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
       <c r="A4" s="16" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C4" s="16" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="D4" s="27" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="E4">
         <v>30</v>
@@ -3955,21 +3964,21 @@
         <v>10</v>
       </c>
       <c r="I4" s="27" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
       <c r="A5" s="16" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B5" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C5" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="D5" s="27" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="E5">
         <v>20</v>
@@ -3984,21 +3993,21 @@
         <v>15</v>
       </c>
       <c r="I5" s="27" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
       <c r="A6" s="16" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B6" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C6" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="D6" s="27" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="E6">
         <v>30</v>
@@ -4013,21 +4022,21 @@
         <v>20</v>
       </c>
       <c r="I6" s="27" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
       <c r="A7" s="16" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B7" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C7" s="16" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="D7" s="27" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="E7">
         <v>20</v>
@@ -4042,21 +4051,21 @@
         <v>15</v>
       </c>
       <c r="I7" s="27" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
       <c r="A8" s="16" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B8" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C8" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="D8" s="27" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="E8">
         <v>30</v>
@@ -4071,21 +4080,21 @@
         <v>20</v>
       </c>
       <c r="I8" s="27" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9">
       <c r="A9" s="16" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B9" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C9" s="16" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="D9" s="27" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="E9">
         <v>30</v>
@@ -4100,21 +4109,21 @@
         <v>10</v>
       </c>
       <c r="I9" s="27" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9">
       <c r="A10" s="16" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B10" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C10" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="D10" s="27" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="E10">
         <v>20</v>
@@ -4129,21 +4138,21 @@
         <v>10</v>
       </c>
       <c r="I10" s="27" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9">
       <c r="A11" s="16" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B11" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C11" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="D11" s="27" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="E11">
         <v>20</v>
@@ -4158,45 +4167,45 @@
         <v>10</v>
       </c>
       <c r="I11" s="27" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9">
       <c r="B14" s="5" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9">
       <c r="B15" s="28" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9">
       <c r="B16" s="5" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:2">
       <c r="B17" s="28" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.3">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="18" spans="2:2">
       <c r="B18" s="28" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="19" spans="2:2" x14ac:dyDescent="0.3">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="19" spans="2:2">
       <c r="B19" s="1"/>
     </row>
-    <row r="20" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:2">
       <c r="B20" s="5" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="21" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:2">
       <c r="B21" s="28" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
     </row>
   </sheetData>
@@ -4211,15 +4220,15 @@
   <dimension ref="A1:I21"/>
   <sheetViews>
     <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17:B21"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.6"/>
   <cols>
-    <col min="2" max="2" width="26.4609375" customWidth="1"/>
+    <col min="2" max="2" width="31.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9">
       <c r="A1" s="4" t="s">
         <v>3</v>
       </c>
@@ -4248,18 +4257,18 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9">
       <c r="A2" s="16" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="B2" s="17" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C2" s="16" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="D2" s="27" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="E2">
         <v>20</v>
@@ -4274,21 +4283,21 @@
         <v>20</v>
       </c>
       <c r="I2" s="27" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
       <c r="A3" s="16" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="B3" s="19" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="C3" s="16" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="D3" s="27" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="E3">
         <v>30</v>
@@ -4303,21 +4312,21 @@
         <v>20</v>
       </c>
       <c r="I3" s="27" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
       <c r="A4" s="16" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C4" s="16" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="D4" s="27" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="E4">
         <v>30</v>
@@ -4332,21 +4341,21 @@
         <v>10</v>
       </c>
       <c r="I4" s="27" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
       <c r="A5" s="16" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B5" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C5" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="D5" s="27" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="E5">
         <v>20</v>
@@ -4361,21 +4370,21 @@
         <v>15</v>
       </c>
       <c r="I5" s="27" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
       <c r="A6" s="16" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B6" t="s">
-        <v>92</v>
+        <v>223</v>
       </c>
       <c r="C6" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="D6" s="27" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="E6">
         <v>30</v>
@@ -4390,21 +4399,21 @@
         <v>20</v>
       </c>
       <c r="I6" s="27" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
       <c r="A7" s="16" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B7" t="s">
-        <v>93</v>
+        <v>225</v>
       </c>
       <c r="C7" s="16" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="D7" s="27" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="E7">
         <v>20</v>
@@ -4419,21 +4428,21 @@
         <v>15</v>
       </c>
       <c r="I7" s="27" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
       <c r="A8" s="16" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B8" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C8" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="D8" s="27" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="E8">
         <v>30</v>
@@ -4448,21 +4457,21 @@
         <v>20</v>
       </c>
       <c r="I8" s="27" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9">
       <c r="A9" s="16" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B9" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C9" s="16" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="D9" s="27" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="E9">
         <v>30</v>
@@ -4477,21 +4486,21 @@
         <v>10</v>
       </c>
       <c r="I9" s="27" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9">
       <c r="A10" s="16" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B10" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C10" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="D10" s="27" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="E10">
         <v>20</v>
@@ -4506,21 +4515,21 @@
         <v>10</v>
       </c>
       <c r="I10" s="27" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9">
       <c r="A11" s="16" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B11" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C11" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="D11" s="27" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="E11">
         <v>20</v>
@@ -4535,45 +4544,45 @@
         <v>10</v>
       </c>
       <c r="I11" s="27" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9">
       <c r="B14" s="5" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9">
       <c r="B15" s="28" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9">
       <c r="B16" s="5" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:2">
       <c r="B17" s="28" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.3">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="18" spans="2:2">
       <c r="B18" s="28" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="19" spans="2:2" x14ac:dyDescent="0.3">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="19" spans="2:2">
       <c r="B19" s="1"/>
     </row>
-    <row r="20" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:2">
       <c r="B20" s="5" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="21" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:2">
       <c r="B21" s="28" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
     </row>
   </sheetData>
@@ -4586,16 +4595,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:I20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="J3" sqref="J3"/>
+    <sheetView zoomScale="150" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.6"/>
   <cols>
-    <col min="2" max="2" width="28.84375" customWidth="1"/>
+    <col min="2" max="2" width="28.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9">
       <c r="A1" s="4" t="s">
         <v>3</v>
       </c>
@@ -4624,15 +4633,15 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9">
       <c r="A2" s="16" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="B2" s="17" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C2" s="16" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="D2" s="16" t="s">
         <v>29</v>
@@ -4653,15 +4662,15 @@
         <v>29</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9">
       <c r="A3" s="16" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="B3" s="17" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C3" s="16" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="D3" s="16" t="s">
         <v>29</v>
@@ -4682,15 +4691,15 @@
         <v>29</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9">
       <c r="A4" s="16" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C4" s="16" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="D4" s="16" t="s">
         <v>29</v>
@@ -4711,15 +4720,15 @@
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9">
       <c r="A5" s="16" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B5" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C5" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="D5" s="16" t="s">
         <v>29</v>
@@ -4740,15 +4749,15 @@
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9">
       <c r="A6" s="16" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B6" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C6" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="D6" s="16" t="s">
         <v>29</v>
@@ -4769,15 +4778,15 @@
         <v>29</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9">
       <c r="A7" s="16" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B7" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C7" s="16" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="D7" s="16" t="s">
         <v>29</v>
@@ -4798,15 +4807,15 @@
         <v>29</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9">
       <c r="A8" s="16" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B8" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C8" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="D8" s="16" t="s">
         <v>29</v>
@@ -4827,15 +4836,15 @@
         <v>29</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9">
       <c r="A9" s="16" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B9" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C9" s="16" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="D9" s="16" t="s">
         <v>29</v>
@@ -4856,15 +4865,15 @@
         <v>29</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9">
       <c r="A10" s="16" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B10" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C10" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="D10" s="16" t="s">
         <v>29</v>
@@ -4885,15 +4894,15 @@
         <v>29</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9">
       <c r="A11" s="16" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B11" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="C11" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="D11" s="16" t="s">
         <v>29</v>
@@ -4914,42 +4923,42 @@
         <v>29</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9">
       <c r="B13" s="5" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9">
       <c r="B14" s="28" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9">
       <c r="B15" s="5" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9">
       <c r="B16" s="28" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.3">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="17" spans="2:2">
       <c r="B17" s="28" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.3">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="18" spans="2:2">
       <c r="B18" s="1"/>
     </row>
-    <row r="19" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:2">
       <c r="B19" s="5" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="20" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:2">
       <c r="B20" s="28" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
     </row>
   </sheetData>
@@ -4962,471 +4971,471 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:C43"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" zoomScale="118" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="C35" sqref="C35"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="118" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.6"/>
   <cols>
-    <col min="2" max="2" width="28.15234375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="68.4609375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="31.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="68.453125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" s="4" customFormat="1">
       <c r="A1" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="15">
+      <c r="A2" s="17" t="s">
         <v>107</v>
       </c>
-      <c r="B1" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="C1" s="5" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="15" x14ac:dyDescent="0.3">
-      <c r="A2" s="17" t="s">
-        <v>108</v>
-      </c>
       <c r="B2" s="17" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C2" s="18" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="15" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" ht="15">
       <c r="A3" s="17" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B3" s="17" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C3" s="18" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="15" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" ht="15">
       <c r="A4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C4" s="12" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" ht="30">
       <c r="A5" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C5" s="12" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="15" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" ht="15">
       <c r="A6" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B6" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C6" s="12" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="15" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" ht="15">
       <c r="A7" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B7" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C7" s="12" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" ht="30">
       <c r="A8" t="s">
+        <v>113</v>
+      </c>
+      <c r="B8" t="s">
+        <v>71</v>
+      </c>
+      <c r="C8" s="12" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="30">
+      <c r="A9" t="s">
         <v>114</v>
       </c>
-      <c r="B8" t="s">
-        <v>72</v>
-      </c>
-      <c r="C8" s="12" t="s">
+      <c r="B9" t="s">
+        <v>148</v>
+      </c>
+      <c r="C9" s="12" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="30">
+      <c r="A10" t="s">
+        <v>115</v>
+      </c>
+      <c r="B10" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" ht="30" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>115</v>
-      </c>
-      <c r="B9" t="s">
-        <v>149</v>
-      </c>
-      <c r="C9" s="12" t="s">
+      <c r="C10" s="12" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="30">
+      <c r="A11" t="s">
+        <v>116</v>
+      </c>
+      <c r="B11" t="s">
+        <v>75</v>
+      </c>
+      <c r="C11" s="12" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="30" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>116</v>
-      </c>
-      <c r="B10" t="s">
-        <v>74</v>
-      </c>
-      <c r="C10" s="12" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" ht="30" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
+    <row r="12" spans="1:3" ht="15">
+      <c r="A12" s="17" t="s">
         <v>117</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B12" s="17" t="s">
         <v>76</v>
-      </c>
-      <c r="C11" s="12" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" ht="15" x14ac:dyDescent="0.3">
-      <c r="A12" s="17" t="s">
-        <v>118</v>
-      </c>
-      <c r="B12" s="17" t="s">
-        <v>77</v>
       </c>
       <c r="C12" s="18" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" ht="30">
       <c r="A13" s="17" t="s">
+        <v>118</v>
+      </c>
+      <c r="B13" s="17" t="s">
+        <v>77</v>
+      </c>
+      <c r="C13" s="18" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="45">
+      <c r="A14" t="s">
         <v>119</v>
       </c>
-      <c r="B13" s="17" t="s">
-        <v>78</v>
-      </c>
-      <c r="C13" s="18" t="s">
+      <c r="B14" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" ht="45" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
+      <c r="C14" s="12" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="15">
+      <c r="A15" t="s">
         <v>120</v>
       </c>
-      <c r="B14" t="s">
-        <v>80</v>
-      </c>
-      <c r="C14" s="12" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" ht="15" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
-        <v>121</v>
-      </c>
       <c r="B15" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C15" s="12" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="15" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" ht="15">
       <c r="A16" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B16" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C16" s="12" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="15" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" ht="15">
       <c r="A17" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B17" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C17" s="12" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="15" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" ht="15">
       <c r="A18" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B18" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C18" s="12" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="15" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" ht="15">
       <c r="A19" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B19" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C19" s="12" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="15" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" ht="15">
       <c r="A20" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B20" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C20" s="12" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="15" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" ht="15">
       <c r="A21" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B21" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C21" s="12" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="15" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3" ht="15">
       <c r="A22" s="17" t="s">
+        <v>127</v>
+      </c>
+      <c r="B22" s="17" t="s">
+        <v>86</v>
+      </c>
+      <c r="C22" s="18" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="15">
+      <c r="A23" s="17" t="s">
         <v>128</v>
       </c>
-      <c r="B22" s="17" t="s">
-        <v>87</v>
-      </c>
-      <c r="C22" s="18" t="s">
+      <c r="B23" s="19" t="s">
+        <v>174</v>
+      </c>
+      <c r="C23" s="18" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="15" x14ac:dyDescent="0.3">
-      <c r="A23" s="17" t="s">
+    <row r="24" spans="1:3" ht="30">
+      <c r="A24" t="s">
         <v>129</v>
       </c>
-      <c r="B23" s="19" t="s">
-        <v>176</v>
-      </c>
-      <c r="C23" s="18" t="s">
+      <c r="B24" t="s">
         <v>89</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" ht="30" x14ac:dyDescent="0.3">
-      <c r="A24" t="s">
-        <v>130</v>
-      </c>
-      <c r="B24" t="s">
-        <v>90</v>
       </c>
       <c r="C24" s="12" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:3" ht="30">
       <c r="A25" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B25" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C25" s="12" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:3" ht="15">
       <c r="A26" t="s">
+        <v>131</v>
+      </c>
+      <c r="B26" t="s">
+        <v>223</v>
+      </c>
+      <c r="C26" s="12" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" ht="15">
+      <c r="A27" t="s">
         <v>132</v>
       </c>
-      <c r="B26" t="s">
-        <v>92</v>
-      </c>
-      <c r="C26" s="12" t="s">
+      <c r="B27" t="s">
+        <v>226</v>
+      </c>
+      <c r="C27" s="12" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" ht="15">
+      <c r="A28" t="s">
+        <v>133</v>
+      </c>
+      <c r="B28" t="s">
+        <v>93</v>
+      </c>
+      <c r="C28" s="12" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="75" x14ac:dyDescent="0.3">
-      <c r="A27" t="s">
-        <v>133</v>
-      </c>
-      <c r="B27" t="s">
-        <v>93</v>
-      </c>
-      <c r="C27" s="12" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" ht="15" x14ac:dyDescent="0.3">
-      <c r="A28" t="s">
+    <row r="29" spans="1:3" ht="15">
+      <c r="A29" t="s">
         <v>134</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B29" t="s">
         <v>94</v>
       </c>
-      <c r="C28" s="12" t="s">
+      <c r="C29" s="12" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" ht="15">
+      <c r="A30" t="s">
+        <v>135</v>
+      </c>
+      <c r="B30" t="s">
+        <v>95</v>
+      </c>
+      <c r="C30" s="12" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="15" x14ac:dyDescent="0.3">
-      <c r="A29" t="s">
-        <v>135</v>
-      </c>
-      <c r="B29" t="s">
-        <v>95</v>
-      </c>
-      <c r="C29" s="12" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" ht="15" x14ac:dyDescent="0.3">
-      <c r="A30" t="s">
+    <row r="31" spans="1:3" ht="15">
+      <c r="A31" t="s">
         <v>136</v>
       </c>
-      <c r="B30" t="s">
+      <c r="B31" t="s">
         <v>96</v>
       </c>
-      <c r="C30" s="12" t="s">
+      <c r="C31" s="12" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="15" x14ac:dyDescent="0.3">
-      <c r="A31" t="s">
+    <row r="32" spans="1:3" ht="15">
+      <c r="A32" s="17" t="s">
         <v>137</v>
       </c>
-      <c r="B31" t="s">
-        <v>97</v>
-      </c>
-      <c r="C31" s="12" t="s">
+      <c r="B32" s="19" t="s">
+        <v>215</v>
+      </c>
+      <c r="C32" s="18" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="15" x14ac:dyDescent="0.3">
-      <c r="A32" s="17" t="s">
+    <row r="33" spans="1:3" ht="15">
+      <c r="A33" s="17" t="s">
         <v>138</v>
       </c>
-      <c r="B32" s="19" t="s">
-        <v>217</v>
-      </c>
-      <c r="C32" s="18" t="s">
+      <c r="B33" s="19" t="s">
+        <v>216</v>
+      </c>
+      <c r="C33" s="18" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="15" x14ac:dyDescent="0.3">
-      <c r="A33" s="17" t="s">
+    <row r="34" spans="1:3" ht="30">
+      <c r="A34" t="s">
         <v>139</v>
       </c>
-      <c r="B33" s="19" t="s">
-        <v>218</v>
-      </c>
-      <c r="C33" s="18" t="s">
+      <c r="B34" s="16" t="s">
+        <v>221</v>
+      </c>
+      <c r="C34" s="12" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="34" spans="1:3" ht="30" x14ac:dyDescent="0.3">
-      <c r="A34" t="s">
+    <row r="35" spans="1:3" ht="30">
+      <c r="A35" t="s">
         <v>140</v>
       </c>
-      <c r="B34" s="16" t="s">
-        <v>223</v>
-      </c>
-      <c r="C34" s="12" t="s">
+      <c r="B35" s="16" t="s">
+        <v>222</v>
+      </c>
+      <c r="C35" s="12" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="35" spans="1:3" ht="30" x14ac:dyDescent="0.3">
-      <c r="A35" t="s">
+    <row r="36" spans="1:3" ht="15">
+      <c r="A36" t="s">
         <v>141</v>
       </c>
-      <c r="B35" s="16" t="s">
-        <v>224</v>
-      </c>
-      <c r="C35" s="12" t="s">
+      <c r="B36" t="s">
+        <v>100</v>
+      </c>
+      <c r="C36" s="12" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="36" spans="1:3" ht="15" x14ac:dyDescent="0.3">
-      <c r="A36" t="s">
+    <row r="37" spans="1:3" ht="15">
+      <c r="A37" t="s">
         <v>142</v>
       </c>
-      <c r="B36" t="s">
+      <c r="B37" t="s">
         <v>101</v>
       </c>
-      <c r="C36" s="12" t="s">
+      <c r="C37" s="12" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="37" spans="1:3" ht="15" x14ac:dyDescent="0.3">
-      <c r="A37" t="s">
+    <row r="38" spans="1:3" ht="30">
+      <c r="A38" t="s">
         <v>143</v>
       </c>
-      <c r="B37" t="s">
+      <c r="B38" t="s">
         <v>102</v>
       </c>
-      <c r="C37" s="12" t="s">
+      <c r="C38" s="12" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="38" spans="1:3" ht="30" x14ac:dyDescent="0.3">
-      <c r="A38" t="s">
+    <row r="39" spans="1:3" ht="15">
+      <c r="A39" t="s">
         <v>144</v>
       </c>
-      <c r="B38" t="s">
+      <c r="B39" t="s">
         <v>103</v>
       </c>
-      <c r="C38" s="12" t="s">
+      <c r="C39" s="12" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="39" spans="1:3" ht="15" x14ac:dyDescent="0.3">
-      <c r="A39" t="s">
+    <row r="40" spans="1:3" ht="30">
+      <c r="A40" t="s">
         <v>145</v>
       </c>
-      <c r="B39" t="s">
+      <c r="B40" t="s">
         <v>104</v>
       </c>
-      <c r="C39" s="12" t="s">
+      <c r="C40" s="12" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="40" spans="1:3" ht="30" x14ac:dyDescent="0.3">
-      <c r="A40" t="s">
+    <row r="41" spans="1:3" ht="30">
+      <c r="A41" t="s">
         <v>146</v>
       </c>
-      <c r="B40" t="s">
-        <v>105</v>
-      </c>
-      <c r="C40" s="12" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" ht="30" x14ac:dyDescent="0.3">
-      <c r="A41" t="s">
-        <v>147</v>
-      </c>
       <c r="B41" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="C41" s="12" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" ht="15" x14ac:dyDescent="0.3">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" ht="15">
       <c r="C42" s="12"/>
     </row>
-    <row r="43" spans="1:3" ht="15" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:3" ht="15">
       <c r="C43" s="12"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Test cases + bugfixes
</commit_message>
<xml_diff>
--- a/Team05Report.xlsx
+++ b/Team05Report.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\samar\Downloads\Scanned pics\New\Assignments\Agile\Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEFC0C45-35E1-4772-862A-228415ED589B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFEB12E9-2DA6-407E-AD74-4538F103369C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" firstSheet="2" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="596" uniqueCount="223">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="610" uniqueCount="228">
   <si>
     <t>Date</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -348,6 +348,9 @@
     <t>Unique families by spouses</t>
   </si>
   <si>
+    <t>Unique first names in families</t>
+  </si>
+  <si>
     <t>Corresponding entries</t>
   </si>
   <si>
@@ -387,12 +390,6 @@
     <t>List upcoming anniversaries</t>
   </si>
   <si>
-    <t>Include input line numbers</t>
-  </si>
-  <si>
-    <t>List line numbers from GEDCOM source file when reporting errors</t>
-  </si>
-  <si>
     <t>List large age differences</t>
   </si>
   <si>
@@ -571,9 +568,6 @@
   </si>
   <si>
     <t>Birth dates of siblings should be more than 8 months apart or less than 2 days apart (twins may be born one day apart, e.g. 11:59 PM and 12:02 AM the following calendar day)</t>
-  </si>
-  <si>
-    <t>All family roles (spouse, child) specified in an individual record should have corresponding entries in the corresponding family records. Likewise, all individual roles (spouse, child) specified in family records should have corresponding entries in the corresponding  individual's records.  I.e. the information in the individual and family records should be consistent.</t>
   </si>
   <si>
     <t>List siblings in families by decreasing age, i.e. oldest siblings first</t>
@@ -752,10 +746,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>Coding</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>Done</t>
     <phoneticPr fontId="6" type="noConversion"/>
   </si>
@@ -808,20 +798,47 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>Coding</t>
+    <t>List living single</t>
     <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
-    <t>Unique child names in families</t>
+    <t>List multiple births</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>Reject Illegitimate Dates</t>
+  </si>
+  <si>
+    <t>Done</t>
+  </si>
+  <si>
+    <t>Reject illegitimate dates</t>
+  </si>
+  <si>
+    <t>All dates should be legitimate dates for the months specified (e.g., 2/30/2015 is not legitimate)</t>
+  </si>
+  <si>
+    <t>List orphans</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>List large age differences</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>Unique first names of childs in families</t>
   </si>
   <si>
     <t>No more than one child with the same name should appear in a family</t>
   </si>
   <si>
-    <t>Unique child first names in families</t>
-  </si>
-  <si>
-    <t>Coding</t>
+    <t>List All births</t>
+  </si>
+  <si>
+    <t>Liat All births</t>
+  </si>
+  <si>
+    <t>List all the birthdays in the GEDCOM File</t>
   </si>
 </sst>
 </file>
@@ -1307,6 +1324,9 @@
                 <c:pt idx="3">
                   <c:v>42313</c:v>
                 </c:pt>
+                <c:pt idx="4">
+                  <c:v>42327</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
@@ -1327,6 +1347,9 @@
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2247,87 +2270,87 @@
     </row>
     <row r="2" spans="1:7">
       <c r="A2" s="20" t="s">
+        <v>175</v>
+      </c>
+      <c r="B2" s="20" t="s">
+        <v>176</v>
+      </c>
+      <c r="C2" s="20" t="s">
         <v>177</v>
       </c>
-      <c r="B2" s="20" t="s">
+      <c r="D2" s="21" t="s">
+        <v>191</v>
+      </c>
+      <c r="E2" s="20" t="s">
         <v>178</v>
-      </c>
-      <c r="C2" s="20" t="s">
-        <v>179</v>
-      </c>
-      <c r="D2" s="21" t="s">
-        <v>193</v>
-      </c>
-      <c r="E2" s="20" t="s">
-        <v>180</v>
       </c>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" s="20" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B3" s="20" t="s">
+        <v>179</v>
+      </c>
+      <c r="C3" s="20" t="s">
+        <v>180</v>
+      </c>
+      <c r="D3" s="21" t="s">
+        <v>192</v>
+      </c>
+      <c r="E3" s="20" t="s">
         <v>181</v>
-      </c>
-      <c r="C3" s="20" t="s">
-        <v>182</v>
-      </c>
-      <c r="D3" s="21" t="s">
-        <v>194</v>
-      </c>
-      <c r="E3" s="20" t="s">
-        <v>183</v>
       </c>
     </row>
     <row r="4" spans="1:7">
       <c r="A4" s="20" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B4" s="20" t="s">
+        <v>182</v>
+      </c>
+      <c r="C4" s="20" t="s">
+        <v>183</v>
+      </c>
+      <c r="D4" s="21" t="s">
+        <v>193</v>
+      </c>
+      <c r="E4" s="20" t="s">
         <v>184</v>
-      </c>
-      <c r="C4" s="20" t="s">
-        <v>185</v>
-      </c>
-      <c r="D4" s="21" t="s">
-        <v>195</v>
-      </c>
-      <c r="E4" s="20" t="s">
-        <v>186</v>
       </c>
     </row>
     <row r="5" spans="1:7">
       <c r="A5" s="20" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B5" s="20" t="s">
+        <v>185</v>
+      </c>
+      <c r="C5" s="20" t="s">
+        <v>186</v>
+      </c>
+      <c r="D5" s="21" t="s">
+        <v>194</v>
+      </c>
+      <c r="E5" s="20" t="s">
         <v>187</v>
-      </c>
-      <c r="C5" s="20" t="s">
-        <v>188</v>
-      </c>
-      <c r="D5" s="21" t="s">
-        <v>196</v>
-      </c>
-      <c r="E5" s="20" t="s">
-        <v>189</v>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c r="A6" s="20" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="B6" s="20" t="s">
+        <v>188</v>
+      </c>
+      <c r="C6" s="20" t="s">
+        <v>189</v>
+      </c>
+      <c r="D6" s="21" t="s">
+        <v>195</v>
+      </c>
+      <c r="E6" s="20" t="s">
         <v>190</v>
-      </c>
-      <c r="C6" s="20" t="s">
-        <v>191</v>
-      </c>
-      <c r="D6" s="21" t="s">
-        <v>197</v>
-      </c>
-      <c r="E6" s="20" t="s">
-        <v>192</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -2338,17 +2361,17 @@
         <v>35</v>
       </c>
       <c r="E9" s="21" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="F9" s="24"/>
       <c r="G9" s="24"/>
     </row>
     <row r="10" spans="1:7">
       <c r="D10" s="24" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="E10" s="25" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="F10" s="24"/>
       <c r="G10" s="24"/>
@@ -2375,17 +2398,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="150" workbookViewId="0">
-      <selection activeCell="G28" sqref="G28"/>
+    <sheetView topLeftCell="A20" zoomScale="150" workbookViewId="0">
+      <selection activeCell="C41" sqref="C41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.6"/>
   <cols>
     <col min="1" max="1" width="5.1796875" customWidth="1"/>
-    <col min="2" max="2" width="9.6328125" customWidth="1"/>
+    <col min="2" max="2" width="9.7265625" customWidth="1"/>
     <col min="3" max="3" width="31" customWidth="1"/>
-    <col min="4" max="4" width="6.6328125" customWidth="1"/>
-    <col min="5" max="5" width="7.6328125" customWidth="1"/>
+    <col min="4" max="4" width="6.7265625" customWidth="1"/>
+    <col min="5" max="5" width="7.7265625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="4" customFormat="1">
@@ -2410,13 +2433,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="16" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="C2" s="17" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D2" s="16" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="E2" t="s">
         <v>29</v>
@@ -2427,13 +2450,13 @@
         <v>2</v>
       </c>
       <c r="B3" s="16" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="C3" s="17" t="s">
         <v>67</v>
       </c>
       <c r="D3" s="16" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="E3" t="s">
         <v>29</v>
@@ -2444,13 +2467,13 @@
         <v>3</v>
       </c>
       <c r="B4" s="16" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="C4" t="s">
         <v>66</v>
       </c>
       <c r="D4" s="16" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="E4" t="s">
         <v>29</v>
@@ -2461,13 +2484,13 @@
         <v>4</v>
       </c>
       <c r="B5" s="16" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C5" t="s">
         <v>68</v>
       </c>
       <c r="D5" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="E5" t="s">
         <v>29</v>
@@ -2478,13 +2501,13 @@
         <v>5</v>
       </c>
       <c r="B6" s="16" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C6" t="s">
         <v>69</v>
       </c>
       <c r="D6" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="E6" t="s">
         <v>29</v>
@@ -2495,13 +2518,13 @@
         <v>6</v>
       </c>
       <c r="B7" s="16" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C7" t="s">
         <v>70</v>
       </c>
       <c r="D7" s="16" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="E7" t="s">
         <v>29</v>
@@ -2512,13 +2535,13 @@
         <v>7</v>
       </c>
       <c r="B8" s="16" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C8" t="s">
         <v>71</v>
       </c>
       <c r="D8" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="E8" t="s">
         <v>29</v>
@@ -2529,13 +2552,13 @@
         <v>8</v>
       </c>
       <c r="B9" s="16" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C9" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D9" s="16" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="E9" t="s">
         <v>29</v>
@@ -2546,13 +2569,13 @@
         <v>9</v>
       </c>
       <c r="B10" s="16" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C10" t="s">
         <v>73</v>
       </c>
       <c r="D10" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="E10" t="s">
         <v>29</v>
@@ -2563,13 +2586,13 @@
         <v>10</v>
       </c>
       <c r="B11" s="16" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C11" t="s">
         <v>75</v>
       </c>
       <c r="D11" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="E11" t="s">
         <v>29</v>
@@ -2580,13 +2603,13 @@
         <v>11</v>
       </c>
       <c r="B12" s="16" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C12" s="17" t="s">
         <v>76</v>
       </c>
       <c r="D12" s="16" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="E12" t="s">
         <v>29</v>
@@ -2597,13 +2620,13 @@
         <v>12</v>
       </c>
       <c r="B13" s="16" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C13" s="17" t="s">
         <v>77</v>
       </c>
       <c r="D13" s="16" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="E13" t="s">
         <v>29</v>
@@ -2614,13 +2637,13 @@
         <v>13</v>
       </c>
       <c r="B14" s="16" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C14" t="s">
         <v>79</v>
       </c>
       <c r="D14" s="16" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="E14" t="s">
         <v>29</v>
@@ -2631,13 +2654,13 @@
         <v>14</v>
       </c>
       <c r="B15" s="16" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C15" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D15" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="E15" t="s">
         <v>29</v>
@@ -2648,13 +2671,13 @@
         <v>15</v>
       </c>
       <c r="B16" s="16" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C16" t="s">
         <v>80</v>
       </c>
       <c r="D16" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="E16" t="s">
         <v>29</v>
@@ -2665,13 +2688,13 @@
         <v>16</v>
       </c>
       <c r="B17" s="16" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C17" t="s">
         <v>81</v>
       </c>
       <c r="D17" s="16" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="E17" t="s">
         <v>29</v>
@@ -2682,13 +2705,13 @@
         <v>17</v>
       </c>
       <c r="B18" s="16" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C18" t="s">
         <v>82</v>
       </c>
       <c r="D18" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="E18" t="s">
         <v>29</v>
@@ -2699,13 +2722,13 @@
         <v>18</v>
       </c>
       <c r="B19" s="16" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C19" t="s">
         <v>83</v>
       </c>
       <c r="D19" s="16" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="E19" t="s">
         <v>29</v>
@@ -2716,13 +2739,13 @@
         <v>19</v>
       </c>
       <c r="B20" s="16" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C20" t="s">
         <v>84</v>
       </c>
       <c r="D20" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="E20" t="s">
         <v>29</v>
@@ -2733,13 +2756,13 @@
         <v>20</v>
       </c>
       <c r="B21" s="16" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C21" t="s">
         <v>85</v>
       </c>
       <c r="D21" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="E21" t="s">
         <v>29</v>
@@ -2750,13 +2773,13 @@
         <v>21</v>
       </c>
       <c r="B22" s="16" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C22" s="17" t="s">
         <v>86</v>
       </c>
       <c r="D22" s="16" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="E22" t="s">
         <v>29</v>
@@ -2767,13 +2790,13 @@
         <v>22</v>
       </c>
       <c r="B23" s="16" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C23" s="19" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="D23" s="16" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="E23" t="s">
         <v>29</v>
@@ -2784,13 +2807,13 @@
         <v>23</v>
       </c>
       <c r="B24" s="16" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C24" t="s">
         <v>89</v>
       </c>
       <c r="D24" s="16" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="E24" t="s">
         <v>29</v>
@@ -2801,13 +2824,13 @@
         <v>24</v>
       </c>
       <c r="B25" s="16" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C25" t="s">
         <v>90</v>
       </c>
       <c r="D25" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="E25" t="s">
         <v>29</v>
@@ -2818,13 +2841,13 @@
         <v>25</v>
       </c>
       <c r="B26" s="16" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C26" t="s">
-        <v>221</v>
+        <v>91</v>
       </c>
       <c r="D26" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="E26" t="s">
         <v>29</v>
@@ -2835,16 +2858,16 @@
         <v>26</v>
       </c>
       <c r="B27" s="16" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C27" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="D27" s="16" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="E27" t="s">
-        <v>222</v>
+        <v>29</v>
       </c>
     </row>
     <row r="28" spans="1:5">
@@ -2852,13 +2875,13 @@
         <v>27</v>
       </c>
       <c r="B28" s="16" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C28" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="D28" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="E28" t="s">
         <v>29</v>
@@ -2869,13 +2892,13 @@
         <v>28</v>
       </c>
       <c r="B29" s="16" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C29" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="D29" s="16" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="E29" t="s">
         <v>29</v>
@@ -2886,13 +2909,13 @@
         <v>29</v>
       </c>
       <c r="B30" s="16" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C30" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D30" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="E30" t="s">
         <v>29</v>
@@ -2903,13 +2926,13 @@
         <v>30</v>
       </c>
       <c r="B31" s="16" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C31" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="D31" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="E31" t="s">
         <v>29</v>
@@ -2920,16 +2943,16 @@
         <v>31</v>
       </c>
       <c r="B32" s="16" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C32" s="17" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="D32" s="16" t="s">
-        <v>173</v>
-      </c>
-      <c r="E32" s="16" t="s">
-        <v>204</v>
+        <v>171</v>
+      </c>
+      <c r="E32" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="33" spans="1:5">
@@ -2937,16 +2960,16 @@
         <v>32</v>
       </c>
       <c r="B33" s="16" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C33" s="17" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="D33" s="16" t="s">
-        <v>169</v>
-      </c>
-      <c r="E33" s="16" t="s">
-        <v>204</v>
+        <v>167</v>
+      </c>
+      <c r="E33" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="34" spans="1:5">
@@ -2954,16 +2977,16 @@
         <v>33</v>
       </c>
       <c r="B34" s="16" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C34" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="D34" s="16" t="s">
-        <v>170</v>
-      </c>
-      <c r="E34" s="16" t="s">
-        <v>204</v>
+        <v>168</v>
+      </c>
+      <c r="E34" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="35" spans="1:5">
@@ -2971,16 +2994,16 @@
         <v>34</v>
       </c>
       <c r="B35" s="16" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C35" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D35" t="s">
-        <v>170</v>
-      </c>
-      <c r="E35" s="16" t="s">
-        <v>204</v>
+        <v>168</v>
+      </c>
+      <c r="E35" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="36" spans="1:5">
@@ -2988,16 +3011,16 @@
         <v>35</v>
       </c>
       <c r="B36" s="16" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C36" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="D36" t="s">
-        <v>171</v>
-      </c>
-      <c r="E36" s="16" t="s">
-        <v>204</v>
+        <v>169</v>
+      </c>
+      <c r="E36" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="37" spans="1:5">
@@ -3005,16 +3028,16 @@
         <v>36</v>
       </c>
       <c r="B37" s="16" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C37" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="D37" s="16" t="s">
-        <v>174</v>
-      </c>
-      <c r="E37" s="16" t="s">
-        <v>204</v>
+        <v>172</v>
+      </c>
+      <c r="E37" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="38" spans="1:5">
@@ -3022,16 +3045,16 @@
         <v>37</v>
       </c>
       <c r="B38" s="16" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C38" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="D38" t="s">
-        <v>168</v>
-      </c>
-      <c r="E38" s="16" t="s">
-        <v>204</v>
+        <v>166</v>
+      </c>
+      <c r="E38" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="39" spans="1:5">
@@ -3039,16 +3062,16 @@
         <v>38</v>
       </c>
       <c r="B39" s="16" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C39" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="D39" s="16" t="s">
-        <v>175</v>
-      </c>
-      <c r="E39" s="16" t="s">
-        <v>204</v>
+        <v>173</v>
+      </c>
+      <c r="E39" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="40" spans="1:5">
@@ -3056,16 +3079,16 @@
         <v>39</v>
       </c>
       <c r="B40" s="16" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C40" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="D40" t="s">
-        <v>172</v>
-      </c>
-      <c r="E40" s="16" t="s">
-        <v>204</v>
+        <v>170</v>
+      </c>
+      <c r="E40" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="41" spans="1:5">
@@ -3073,16 +3096,16 @@
         <v>40</v>
       </c>
       <c r="B41" s="16" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C41" t="s">
-        <v>104</v>
+        <v>217</v>
       </c>
       <c r="D41" t="s">
-        <v>172</v>
-      </c>
-      <c r="E41" s="16" t="s">
-        <v>204</v>
+        <v>170</v>
+      </c>
+      <c r="E41" t="s">
+        <v>218</v>
       </c>
     </row>
   </sheetData>
@@ -3105,44 +3128,44 @@
     <col min="1" max="1" width="10.81640625" style="7"/>
     <col min="2" max="2" width="9.453125" customWidth="1"/>
     <col min="3" max="3" width="15.81640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.36328125" customWidth="1"/>
+    <col min="4" max="4" width="12.26953125" customWidth="1"/>
     <col min="5" max="5" width="6.81640625" customWidth="1"/>
     <col min="6" max="6" width="12.453125" style="9" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" s="7" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="2" spans="1:7">
       <c r="A2" s="7" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" s="7" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="5" spans="1:7">
       <c r="A5" s="7" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c r="A6" s="7" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="7" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="14" spans="1:7" s="4" customFormat="1">
       <c r="A14" s="4" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B14" s="3" t="s">
         <v>0</v>
@@ -3165,7 +3188,7 @@
     </row>
     <row r="15" spans="1:7">
       <c r="A15" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B15" s="13">
         <v>41065</v>
@@ -3181,7 +3204,7 @@
     </row>
     <row r="16" spans="1:7">
       <c r="A16" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B16" s="13">
         <v>41078</v>
@@ -3206,7 +3229,7 @@
     </row>
     <row r="17" spans="1:7">
       <c r="A17" s="7" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B17" s="13">
         <v>41092</v>
@@ -3231,7 +3254,7 @@
     </row>
     <row r="18" spans="1:7">
       <c r="A18" s="7" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B18" s="13">
         <v>41106</v>
@@ -3256,7 +3279,7 @@
     </row>
     <row r="19" spans="1:7">
       <c r="A19" s="7" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B19" s="13">
         <v>41120</v>
@@ -3289,10 +3312,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.6"/>
@@ -3301,7 +3324,7 @@
     <col min="2" max="2" width="24.453125" customWidth="1"/>
     <col min="3" max="3" width="17.81640625" customWidth="1"/>
     <col min="4" max="4" width="11.1796875" customWidth="1"/>
-    <col min="5" max="5" width="13.6328125" customWidth="1"/>
+    <col min="5" max="5" width="13.7265625" customWidth="1"/>
     <col min="6" max="6" width="12.453125" style="9" customWidth="1"/>
   </cols>
   <sheetData>
@@ -3398,6 +3421,27 @@
       <c r="F5" s="9">
         <f>(D5-D2)/E5*60</f>
         <v>48</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" s="2">
+        <v>42327</v>
+      </c>
+      <c r="B6">
+        <v>0</v>
+      </c>
+      <c r="C6">
+        <v>10</v>
+      </c>
+      <c r="D6">
+        <v>120</v>
+      </c>
+      <c r="E6">
+        <v>120</v>
+      </c>
+      <c r="F6" s="9">
+        <f>(D6-D2)/E6*60</f>
+        <v>60</v>
       </c>
     </row>
   </sheetData>
@@ -3418,11 +3462,11 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.6"/>
   <cols>
-    <col min="1" max="1" width="7.6328125" customWidth="1"/>
+    <col min="1" max="1" width="7.7265625" customWidth="1"/>
     <col min="2" max="2" width="24.453125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="12.6328125" customWidth="1"/>
+    <col min="3" max="3" width="12.7265625" customWidth="1"/>
     <col min="4" max="4" width="20.81640625" customWidth="1"/>
-    <col min="5" max="5" width="14.6328125" customWidth="1"/>
+    <col min="5" max="5" width="14.7265625" customWidth="1"/>
     <col min="6" max="6" width="11.81640625" customWidth="1"/>
     <col min="7" max="7" width="12.81640625" customWidth="1"/>
     <col min="8" max="8" width="18" customWidth="1"/>
@@ -3460,16 +3504,16 @@
     </row>
     <row r="2" spans="1:9">
       <c r="A2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C2" s="16" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="D2" s="27" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="E2">
         <v>50</v>
@@ -3489,16 +3533,16 @@
     </row>
     <row r="3" spans="1:9">
       <c r="A3" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>67</v>
       </c>
       <c r="C3" s="16" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="D3" s="27" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="E3">
         <v>50</v>
@@ -3518,16 +3562,16 @@
     </row>
     <row r="4" spans="1:9">
       <c r="A4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>66</v>
       </c>
       <c r="C4" s="16" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="D4" s="27" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="E4">
         <v>50</v>
@@ -3547,16 +3591,16 @@
     </row>
     <row r="5" spans="1:9">
       <c r="A5" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>68</v>
       </c>
       <c r="C5" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="D5" s="27" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="E5">
         <v>60</v>
@@ -3576,16 +3620,16 @@
     </row>
     <row r="6" spans="1:9">
       <c r="A6" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>69</v>
       </c>
       <c r="C6" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="D6" s="27" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="E6">
         <v>50</v>
@@ -3605,16 +3649,16 @@
     </row>
     <row r="7" spans="1:9">
       <c r="A7" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>70</v>
       </c>
       <c r="C7" s="16" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="D7" s="27" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="E7">
         <v>70</v>
@@ -3634,16 +3678,16 @@
     </row>
     <row r="8" spans="1:9">
       <c r="A8" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>71</v>
       </c>
       <c r="C8" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="D8" s="27" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="E8">
         <v>60</v>
@@ -3663,16 +3707,16 @@
     </row>
     <row r="9" spans="1:9" ht="25.2">
       <c r="A9" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C9" s="16" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="D9" s="27" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="E9">
         <v>50</v>
@@ -3692,16 +3736,16 @@
     </row>
     <row r="10" spans="1:9">
       <c r="A10" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B10" t="s">
         <v>73</v>
       </c>
       <c r="C10" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="D10" s="27" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="E10">
         <v>40</v>
@@ -3721,16 +3765,16 @@
     </row>
     <row r="11" spans="1:9">
       <c r="A11" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B11" t="s">
         <v>75</v>
       </c>
       <c r="C11" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="D11" s="27" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="E11">
         <v>50</v>
@@ -3755,7 +3799,7 @@
     </row>
     <row r="15" spans="1:9">
       <c r="B15" s="28" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="I15" s="7"/>
     </row>
@@ -3766,12 +3810,12 @@
     </row>
     <row r="17" spans="2:2">
       <c r="B17" s="28" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
     </row>
     <row r="18" spans="2:2">
       <c r="B18" s="28" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
     </row>
     <row r="20" spans="2:2">
@@ -3781,7 +3825,7 @@
     </row>
     <row r="21" spans="2:2">
       <c r="B21" s="28" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
     </row>
   </sheetData>
@@ -3796,7 +3840,7 @@
   <dimension ref="A1:I21"/>
   <sheetViews>
     <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.6"/>
@@ -3838,16 +3882,16 @@
     </row>
     <row r="2" spans="1:9">
       <c r="A2" s="16" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="B2" s="17" t="s">
         <v>76</v>
       </c>
       <c r="C2" s="16" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="D2" s="27" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="E2">
         <v>20</v>
@@ -3862,21 +3906,21 @@
         <v>20</v>
       </c>
       <c r="I2" s="27" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
     </row>
     <row r="3" spans="1:9">
       <c r="A3" s="16" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="B3" s="17" t="s">
         <v>77</v>
       </c>
       <c r="C3" s="16" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="D3" s="27" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="E3">
         <v>30</v>
@@ -3891,21 +3935,21 @@
         <v>20</v>
       </c>
       <c r="I3" s="27" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
     </row>
     <row r="4" spans="1:9">
       <c r="A4" s="16" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B4" t="s">
         <v>79</v>
       </c>
       <c r="C4" s="16" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="D4" s="27" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="E4">
         <v>30</v>
@@ -3920,21 +3964,21 @@
         <v>10</v>
       </c>
       <c r="I4" s="27" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
     </row>
     <row r="5" spans="1:9">
       <c r="A5" s="16" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B5" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C5" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="D5" s="27" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="E5">
         <v>20</v>
@@ -3949,21 +3993,21 @@
         <v>15</v>
       </c>
       <c r="I5" s="27" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
     </row>
     <row r="6" spans="1:9">
       <c r="A6" s="16" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B6" t="s">
         <v>80</v>
       </c>
       <c r="C6" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="D6" s="27" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="E6">
         <v>30</v>
@@ -3978,21 +4022,21 @@
         <v>20</v>
       </c>
       <c r="I6" s="27" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
     </row>
     <row r="7" spans="1:9">
       <c r="A7" s="16" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B7" t="s">
         <v>81</v>
       </c>
       <c r="C7" s="16" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="D7" s="27" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="E7">
         <v>20</v>
@@ -4007,21 +4051,21 @@
         <v>15</v>
       </c>
       <c r="I7" s="27" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
     </row>
     <row r="8" spans="1:9">
       <c r="A8" s="16" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B8" t="s">
         <v>82</v>
       </c>
       <c r="C8" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="D8" s="27" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="E8">
         <v>30</v>
@@ -4036,21 +4080,21 @@
         <v>20</v>
       </c>
       <c r="I8" s="27" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
     </row>
     <row r="9" spans="1:9">
       <c r="A9" s="16" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B9" t="s">
         <v>83</v>
       </c>
       <c r="C9" s="16" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="D9" s="27" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="E9">
         <v>30</v>
@@ -4065,21 +4109,21 @@
         <v>10</v>
       </c>
       <c r="I9" s="27" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
     </row>
     <row r="10" spans="1:9">
       <c r="A10" s="16" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B10" t="s">
         <v>84</v>
       </c>
       <c r="C10" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="D10" s="27" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="E10">
         <v>20</v>
@@ -4094,21 +4138,21 @@
         <v>10</v>
       </c>
       <c r="I10" s="27" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
     </row>
     <row r="11" spans="1:9">
       <c r="A11" s="16" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B11" t="s">
         <v>85</v>
       </c>
       <c r="C11" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="D11" s="27" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="E11">
         <v>20</v>
@@ -4123,7 +4167,7 @@
         <v>10</v>
       </c>
       <c r="I11" s="27" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
     </row>
     <row r="14" spans="1:9">
@@ -4133,7 +4177,7 @@
     </row>
     <row r="15" spans="1:9">
       <c r="B15" s="28" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
     </row>
     <row r="16" spans="1:9">
@@ -4143,12 +4187,12 @@
     </row>
     <row r="17" spans="2:2">
       <c r="B17" s="28" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
     </row>
     <row r="18" spans="2:2">
       <c r="B18" s="28" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
     </row>
     <row r="19" spans="2:2">
@@ -4161,7 +4205,7 @@
     </row>
     <row r="21" spans="2:2">
       <c r="B21" s="28" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
     </row>
   </sheetData>
@@ -4175,13 +4219,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:I21"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" zoomScale="150" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+    <sheetView zoomScale="150" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.6"/>
   <cols>
-    <col min="2" max="2" width="38.08984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
@@ -4215,16 +4259,16 @@
     </row>
     <row r="2" spans="1:9">
       <c r="A2" s="16" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="B2" s="17" t="s">
         <v>86</v>
       </c>
       <c r="C2" s="16" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="D2" s="27" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="E2">
         <v>20</v>
@@ -4239,21 +4283,21 @@
         <v>20</v>
       </c>
       <c r="I2" s="27" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
     </row>
     <row r="3" spans="1:9">
       <c r="A3" s="16" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="B3" s="19" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="C3" s="16" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="D3" s="27" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="E3">
         <v>30</v>
@@ -4268,21 +4312,21 @@
         <v>20</v>
       </c>
       <c r="I3" s="27" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
     </row>
     <row r="4" spans="1:9">
       <c r="A4" s="16" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B4" t="s">
         <v>89</v>
       </c>
       <c r="C4" s="16" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="D4" s="27" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="E4">
         <v>30</v>
@@ -4297,21 +4341,21 @@
         <v>10</v>
       </c>
       <c r="I4" s="27" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
     </row>
     <row r="5" spans="1:9">
       <c r="A5" s="16" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B5" t="s">
         <v>90</v>
       </c>
       <c r="C5" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="D5" s="27" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="E5">
         <v>20</v>
@@ -4326,21 +4370,21 @@
         <v>15</v>
       </c>
       <c r="I5" s="27" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
     </row>
     <row r="6" spans="1:9">
       <c r="A6" s="16" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B6" t="s">
-        <v>219</v>
+        <v>223</v>
       </c>
       <c r="C6" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="D6" s="27" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="E6">
         <v>30</v>
@@ -4355,21 +4399,21 @@
         <v>20</v>
       </c>
       <c r="I6" s="27" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
     </row>
     <row r="7" spans="1:9">
       <c r="A7" s="16" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B7" t="s">
-        <v>91</v>
+        <v>225</v>
       </c>
       <c r="C7" s="16" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="D7" s="27" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="E7">
         <v>20</v>
@@ -4384,21 +4428,21 @@
         <v>15</v>
       </c>
       <c r="I7" s="27" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
     </row>
     <row r="8" spans="1:9">
       <c r="A8" s="16" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B8" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C8" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="D8" s="27" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="E8">
         <v>30</v>
@@ -4413,21 +4457,21 @@
         <v>20</v>
       </c>
       <c r="I8" s="27" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
     </row>
     <row r="9" spans="1:9">
       <c r="A9" s="16" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B9" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="C9" s="16" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="D9" s="27" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="E9">
         <v>30</v>
@@ -4442,21 +4486,21 @@
         <v>10</v>
       </c>
       <c r="I9" s="27" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
     </row>
     <row r="10" spans="1:9">
       <c r="A10" s="16" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B10" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C10" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="D10" s="27" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="E10">
         <v>20</v>
@@ -4471,21 +4515,21 @@
         <v>10</v>
       </c>
       <c r="I10" s="27" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
     </row>
     <row r="11" spans="1:9">
       <c r="A11" s="16" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B11" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="C11" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="D11" s="27" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="E11">
         <v>20</v>
@@ -4500,7 +4544,7 @@
         <v>10</v>
       </c>
       <c r="I11" s="27" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
     </row>
     <row r="14" spans="1:9">
@@ -4510,7 +4554,7 @@
     </row>
     <row r="15" spans="1:9">
       <c r="B15" s="28" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
     </row>
     <row r="16" spans="1:9">
@@ -4520,12 +4564,12 @@
     </row>
     <row r="17" spans="2:2">
       <c r="B17" s="28" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
     </row>
     <row r="18" spans="2:2">
       <c r="B18" s="28" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
     </row>
     <row r="19" spans="2:2">
@@ -4538,7 +4582,7 @@
     </row>
     <row r="21" spans="2:2">
       <c r="B21" s="28" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
     </row>
   </sheetData>
@@ -4552,7 +4596,7 @@
   <dimension ref="A1:I20"/>
   <sheetViews>
     <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.6"/>
@@ -4591,36 +4635,45 @@
     </row>
     <row r="2" spans="1:9">
       <c r="A2" s="16" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="B2" s="17" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C2" s="16" t="s">
-        <v>173</v>
-      </c>
-      <c r="D2" s="27" t="s">
-        <v>218</v>
+        <v>171</v>
+      </c>
+      <c r="D2" s="16" t="s">
+        <v>29</v>
       </c>
       <c r="E2">
         <v>20</v>
       </c>
       <c r="F2">
         <v>20</v>
+      </c>
+      <c r="G2">
+        <v>12</v>
+      </c>
+      <c r="H2">
+        <v>15</v>
+      </c>
+      <c r="I2" s="16" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:9">
       <c r="A3" s="16" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="B3" s="17" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="C3" s="16" t="s">
-        <v>169</v>
-      </c>
-      <c r="D3" s="27" t="s">
-        <v>218</v>
+        <v>167</v>
+      </c>
+      <c r="D3" s="16" t="s">
+        <v>29</v>
       </c>
       <c r="E3">
         <v>30</v>
@@ -4628,19 +4681,28 @@
       <c r="F3">
         <v>30</v>
       </c>
+      <c r="G3">
+        <v>11</v>
+      </c>
+      <c r="H3">
+        <v>15</v>
+      </c>
+      <c r="I3" s="16" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="4" spans="1:9">
       <c r="A4" s="16" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B4" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C4" s="16" t="s">
-        <v>170</v>
-      </c>
-      <c r="D4" s="27" t="s">
-        <v>218</v>
+        <v>168</v>
+      </c>
+      <c r="D4" s="16" t="s">
+        <v>29</v>
       </c>
       <c r="E4">
         <v>30</v>
@@ -4648,19 +4710,28 @@
       <c r="F4">
         <v>30</v>
       </c>
+      <c r="G4">
+        <v>12</v>
+      </c>
+      <c r="H4">
+        <v>10</v>
+      </c>
+      <c r="I4" s="16" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="5" spans="1:9">
       <c r="A5" s="16" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B5" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C5" t="s">
-        <v>170</v>
-      </c>
-      <c r="D5" s="27" t="s">
-        <v>218</v>
+        <v>168</v>
+      </c>
+      <c r="D5" s="16" t="s">
+        <v>29</v>
       </c>
       <c r="E5">
         <v>20</v>
@@ -4668,19 +4739,28 @@
       <c r="F5">
         <v>30</v>
       </c>
+      <c r="G5">
+        <v>12</v>
+      </c>
+      <c r="H5">
+        <v>30</v>
+      </c>
+      <c r="I5" s="16" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="6" spans="1:9">
       <c r="A6" s="16" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B6" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="C6" t="s">
-        <v>171</v>
-      </c>
-      <c r="D6" s="27" t="s">
-        <v>218</v>
+        <v>169</v>
+      </c>
+      <c r="D6" s="16" t="s">
+        <v>29</v>
       </c>
       <c r="E6">
         <v>30</v>
@@ -4688,39 +4768,57 @@
       <c r="F6">
         <v>30</v>
       </c>
+      <c r="G6">
+        <v>10</v>
+      </c>
+      <c r="H6">
+        <v>20</v>
+      </c>
+      <c r="I6" s="16" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="7" spans="1:9">
       <c r="A7" s="16" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B7" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C7" s="16" t="s">
-        <v>174</v>
-      </c>
-      <c r="D7" s="27" t="s">
-        <v>218</v>
+        <v>172</v>
+      </c>
+      <c r="D7" s="16" t="s">
+        <v>29</v>
       </c>
       <c r="E7">
         <v>20</v>
       </c>
       <c r="F7">
         <v>20</v>
+      </c>
+      <c r="G7">
+        <v>12</v>
+      </c>
+      <c r="H7">
+        <v>15</v>
+      </c>
+      <c r="I7" s="16" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="8" spans="1:9">
       <c r="A8" s="16" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B8" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C8" t="s">
-        <v>168</v>
-      </c>
-      <c r="D8" s="27" t="s">
-        <v>218</v>
+        <v>166</v>
+      </c>
+      <c r="D8" s="16" t="s">
+        <v>29</v>
       </c>
       <c r="E8">
         <v>30</v>
@@ -4728,19 +4826,28 @@
       <c r="F8">
         <v>20</v>
       </c>
+      <c r="G8">
+        <v>12</v>
+      </c>
+      <c r="H8">
+        <v>20</v>
+      </c>
+      <c r="I8" s="16" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="9" spans="1:9">
       <c r="A9" s="16" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B9" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="C9" s="16" t="s">
-        <v>175</v>
-      </c>
-      <c r="D9" s="27" t="s">
-        <v>218</v>
+        <v>173</v>
+      </c>
+      <c r="D9" s="16" t="s">
+        <v>29</v>
       </c>
       <c r="E9">
         <v>30</v>
@@ -4748,45 +4855,72 @@
       <c r="F9">
         <v>20</v>
       </c>
+      <c r="G9">
+        <v>15</v>
+      </c>
+      <c r="H9">
+        <v>10</v>
+      </c>
+      <c r="I9" s="16" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="10" spans="1:9">
       <c r="A10" s="16" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B10" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C10" t="s">
-        <v>172</v>
-      </c>
-      <c r="D10" s="27" t="s">
-        <v>218</v>
+        <v>170</v>
+      </c>
+      <c r="D10" s="16" t="s">
+        <v>29</v>
       </c>
       <c r="E10">
         <v>20</v>
       </c>
       <c r="F10">
         <v>20</v>
+      </c>
+      <c r="G10">
+        <v>13</v>
+      </c>
+      <c r="H10">
+        <v>10</v>
+      </c>
+      <c r="I10" s="16" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="11" spans="1:9">
       <c r="A11" s="16" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B11" t="s">
-        <v>104</v>
+        <v>217</v>
       </c>
       <c r="C11" t="s">
-        <v>172</v>
-      </c>
-      <c r="D11" s="27" t="s">
-        <v>218</v>
+        <v>170</v>
+      </c>
+      <c r="D11" s="16" t="s">
+        <v>29</v>
       </c>
       <c r="E11">
         <v>20</v>
       </c>
       <c r="F11">
         <v>20</v>
+      </c>
+      <c r="G11">
+        <v>11</v>
+      </c>
+      <c r="H11">
+        <v>10</v>
+      </c>
+      <c r="I11" s="16" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="13" spans="1:9">
@@ -4795,7 +4929,9 @@
       </c>
     </row>
     <row r="14" spans="1:9">
-      <c r="B14" s="28"/>
+      <c r="B14" s="28" t="s">
+        <v>212</v>
+      </c>
     </row>
     <row r="15" spans="1:9">
       <c r="B15" s="5" t="s">
@@ -4803,10 +4939,14 @@
       </c>
     </row>
     <row r="16" spans="1:9">
-      <c r="B16" s="28"/>
+      <c r="B16" s="28" t="s">
+        <v>204</v>
+      </c>
     </row>
     <row r="17" spans="2:2">
-      <c r="B17" s="28"/>
+      <c r="B17" s="28" t="s">
+        <v>205</v>
+      </c>
     </row>
     <row r="18" spans="2:2">
       <c r="B18" s="1"/>
@@ -4817,7 +4957,9 @@
       </c>
     </row>
     <row r="20" spans="2:2">
-      <c r="B20" s="28"/>
+      <c r="B20" s="28" t="s">
+        <v>206</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
@@ -4829,19 +4971,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:C43"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" zoomScale="118" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="118" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.6"/>
   <cols>
-    <col min="2" max="2" width="37.54296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.81640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="68.453125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" s="4" customFormat="1">
       <c r="A1" s="4" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>64</v>
@@ -4852,10 +4994,10 @@
     </row>
     <row r="2" spans="1:3" ht="15">
       <c r="A2" s="17" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B2" s="17" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C2" s="18" t="s">
         <v>36</v>
@@ -4863,7 +5005,7 @@
     </row>
     <row r="3" spans="1:3" ht="15">
       <c r="A3" s="17" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B3" s="17" t="s">
         <v>67</v>
@@ -4874,7 +5016,7 @@
     </row>
     <row r="4" spans="1:3" ht="15">
       <c r="A4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B4" t="s">
         <v>66</v>
@@ -4885,7 +5027,7 @@
     </row>
     <row r="5" spans="1:3" ht="30">
       <c r="A5" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B5" t="s">
         <v>68</v>
@@ -4896,7 +5038,7 @@
     </row>
     <row r="6" spans="1:3" ht="15">
       <c r="A6" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B6" t="s">
         <v>69</v>
@@ -4907,7 +5049,7 @@
     </row>
     <row r="7" spans="1:3" ht="15">
       <c r="A7" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B7" t="s">
         <v>70</v>
@@ -4918,7 +5060,7 @@
     </row>
     <row r="8" spans="1:3" ht="30">
       <c r="A8" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B8" t="s">
         <v>71</v>
@@ -4929,18 +5071,18 @@
     </row>
     <row r="9" spans="1:3" ht="30">
       <c r="A9" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B9" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C9" s="12" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="30">
       <c r="A10" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B10" t="s">
         <v>73</v>
@@ -4951,18 +5093,18 @@
     </row>
     <row r="11" spans="1:3" ht="30">
       <c r="A11" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B11" t="s">
         <v>75</v>
       </c>
       <c r="C11" s="12" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="15">
       <c r="A12" s="17" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B12" s="17" t="s">
         <v>76</v>
@@ -4973,7 +5115,7 @@
     </row>
     <row r="13" spans="1:3" ht="30">
       <c r="A13" s="17" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B13" s="17" t="s">
         <v>77</v>
@@ -4984,21 +5126,21 @@
     </row>
     <row r="14" spans="1:3" ht="45">
       <c r="A14" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B14" t="s">
         <v>79</v>
       </c>
       <c r="C14" s="12" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="15">
       <c r="A15" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B15" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C15" s="12" t="s">
         <v>43</v>
@@ -5006,7 +5148,7 @@
     </row>
     <row r="16" spans="1:3" ht="15">
       <c r="A16" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B16" t="s">
         <v>80</v>
@@ -5017,7 +5159,7 @@
     </row>
     <row r="17" spans="1:3" ht="15">
       <c r="A17" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B17" t="s">
         <v>81</v>
@@ -5028,7 +5170,7 @@
     </row>
     <row r="18" spans="1:3" ht="15">
       <c r="A18" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B18" t="s">
         <v>82</v>
@@ -5039,7 +5181,7 @@
     </row>
     <row r="19" spans="1:3" ht="15">
       <c r="A19" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B19" t="s">
         <v>83</v>
@@ -5050,7 +5192,7 @@
     </row>
     <row r="20" spans="1:3" ht="15">
       <c r="A20" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B20" t="s">
         <v>84</v>
@@ -5061,7 +5203,7 @@
     </row>
     <row r="21" spans="1:3" ht="15">
       <c r="A21" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B21" t="s">
         <v>85</v>
@@ -5072,7 +5214,7 @@
     </row>
     <row r="22" spans="1:3" ht="15">
       <c r="A22" s="17" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B22" s="17" t="s">
         <v>86</v>
@@ -5083,10 +5225,10 @@
     </row>
     <row r="23" spans="1:3" ht="15">
       <c r="A23" s="17" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B23" s="19" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="C23" s="18" t="s">
         <v>88</v>
@@ -5094,7 +5236,7 @@
     </row>
     <row r="24" spans="1:3" ht="30">
       <c r="A24" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B24" t="s">
         <v>89</v>
@@ -5105,7 +5247,7 @@
     </row>
     <row r="25" spans="1:3" ht="30">
       <c r="A25" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B25" t="s">
         <v>90</v>
@@ -5116,32 +5258,32 @@
     </row>
     <row r="26" spans="1:3" ht="15">
       <c r="A26" t="s">
+        <v>131</v>
+      </c>
+      <c r="B26" t="s">
+        <v>223</v>
+      </c>
+      <c r="C26" s="12" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" ht="15">
+      <c r="A27" t="s">
         <v>132</v>
       </c>
-      <c r="B26" t="s">
-        <v>219</v>
-      </c>
-      <c r="C26" s="12" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" ht="75">
-      <c r="A27" t="s">
-        <v>133</v>
-      </c>
       <c r="B27" t="s">
-        <v>91</v>
+        <v>226</v>
       </c>
       <c r="C27" s="12" t="s">
-        <v>166</v>
+        <v>227</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="15">
       <c r="A28" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B28" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C28" s="12" t="s">
         <v>52</v>
@@ -5149,21 +5291,21 @@
     </row>
     <row r="29" spans="1:3" ht="15">
       <c r="A29" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B29" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="C29" s="12" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="15">
       <c r="A30" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B30" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C30" s="12" t="s">
         <v>53</v>
@@ -5171,10 +5313,10 @@
     </row>
     <row r="31" spans="1:3" ht="15">
       <c r="A31" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B31" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="C31" s="12" t="s">
         <v>54</v>
@@ -5182,10 +5324,10 @@
     </row>
     <row r="32" spans="1:3" ht="15">
       <c r="A32" s="17" t="s">
-        <v>138</v>
-      </c>
-      <c r="B32" s="17" t="s">
-        <v>96</v>
+        <v>137</v>
+      </c>
+      <c r="B32" s="19" t="s">
+        <v>215</v>
       </c>
       <c r="C32" s="18" t="s">
         <v>55</v>
@@ -5193,10 +5335,10 @@
     </row>
     <row r="33" spans="1:3" ht="15">
       <c r="A33" s="17" t="s">
-        <v>139</v>
-      </c>
-      <c r="B33" s="17" t="s">
-        <v>97</v>
+        <v>138</v>
+      </c>
+      <c r="B33" s="19" t="s">
+        <v>216</v>
       </c>
       <c r="C33" s="18" t="s">
         <v>56</v>
@@ -5204,10 +5346,10 @@
     </row>
     <row r="34" spans="1:3" ht="30">
       <c r="A34" t="s">
-        <v>140</v>
-      </c>
-      <c r="B34" t="s">
-        <v>98</v>
+        <v>139</v>
+      </c>
+      <c r="B34" s="16" t="s">
+        <v>221</v>
       </c>
       <c r="C34" s="12" t="s">
         <v>57</v>
@@ -5215,10 +5357,10 @@
     </row>
     <row r="35" spans="1:3" ht="30">
       <c r="A35" t="s">
-        <v>141</v>
-      </c>
-      <c r="B35" t="s">
-        <v>106</v>
+        <v>140</v>
+      </c>
+      <c r="B35" s="16" t="s">
+        <v>222</v>
       </c>
       <c r="C35" s="12" t="s">
         <v>58</v>
@@ -5226,10 +5368,10 @@
     </row>
     <row r="36" spans="1:3" ht="15">
       <c r="A36" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B36" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="C36" s="12" t="s">
         <v>59</v>
@@ -5237,10 +5379,10 @@
     </row>
     <row r="37" spans="1:3" ht="15">
       <c r="A37" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B37" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C37" s="12" t="s">
         <v>60</v>
@@ -5248,10 +5390,10 @@
     </row>
     <row r="38" spans="1:3" ht="30">
       <c r="A38" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B38" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C38" s="12" t="s">
         <v>61</v>
@@ -5259,10 +5401,10 @@
     </row>
     <row r="39" spans="1:3" ht="15">
       <c r="A39" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B39" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="C39" s="12" t="s">
         <v>62</v>
@@ -5270,24 +5412,24 @@
     </row>
     <row r="40" spans="1:3" ht="30">
       <c r="A40" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B40" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C40" s="12" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="41" spans="1:3" ht="15">
+    <row r="41" spans="1:3" ht="30">
       <c r="A41" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B41" t="s">
-        <v>104</v>
+        <v>219</v>
       </c>
       <c r="C41" s="12" t="s">
-        <v>105</v>
+        <v>220</v>
       </c>
     </row>
     <row r="42" spans="1:3" ht="15">
@@ -5299,6 +5441,6 @@
   </sheetData>
   <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>